<commit_message>
Add new session and speaker details for Armen Vardanyan; fix title formatting
</commit_message>
<xml_diff>
--- a/public/devfest-armenia-2025-flattened-sessions.xlsx
+++ b/public/devfest-armenia-2025-flattened-sessions.xlsx
@@ -7,11 +7,16 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="3U3RRnnZISOg2CxmXwC8bfIO1FZhGfQOys4rEufgizc="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>Session Id</t>
   </si>
@@ -70,7 +75,7 @@
     <t>Profile Picture</t>
   </si>
   <si>
-    <t>Agent  Development Kit Deep Dive [WORKSHOP]</t>
+    <t>Agent Development Kit Deep Dive [WORKSHOP]</t>
   </si>
   <si>
     <t>From Initialization to Ideation to Prompting to Deployment. All of these and the intermediate steps will be covered in the creation of your own Agent application. We all know about AI, but this is much more than that, it is making sure the AI is deployed and available in the most consistent way possible with all the requirements for application development including version control, testing and scaling being covered. You will be given credits to follow along on the workshop.</t>
@@ -82,7 +87,7 @@
     <t>ankur.roy@onlinepartner.se</t>
   </si>
   <si>
-    <t/>
+    <t>Wokshop</t>
   </si>
   <si>
     <t>8ca460b2-bb7b-4e0a-bc41-7a7ddcb2dda3</t>
@@ -107,8 +112,8 @@
   </si>
   <si>
     <t>We all know AI can auto-generate components, codes, and a bunch of other stuff to help us work faster, but the real question is: should 80% of our work be done by AI (is this even possible for high-quality work), and how much automation is truly too much?
-I'm sharing a practical look at how I'm using AI in the product creation workflow, from actionable tricks that get better product workflow and documentation to the real, often-unspoken problem of maintaining design authority and preventing our essential human skills from slowing down. 
-This session is for everyone ready to stop listening to the hype and find the necessary balance between AI speed and lasting quality.</t>
+ I'm sharing a practical look at how I'm using AI in the product creation workflow, from actionable tricks that get better product workflow and documentation to the real, often-unspoken problem of maintaining design authority and preventing our essential human skills from slowing down. 
+ This session is for everyone ready to stop listening to the hype and find the necessary balance between AI speed and lasting quality.</t>
   </si>
   <si>
     <t>Seda Sahakyan</t>
@@ -117,82 +122,113 @@
     <t>seda.design05@gmail.com</t>
   </si>
   <si>
+    <t>Hall A</t>
+  </si>
+  <si>
+    <t>695c0a43-6758-4801-bb70-bb1e447b4df2</t>
+  </si>
+  <si>
+    <t>Seda</t>
+  </si>
+  <si>
+    <t>Sahakyan</t>
+  </si>
+  <si>
+    <t>Product Designer, iGameMedia</t>
+  </si>
+  <si>
+    <t>Seda, a product designer crafting digital experiences since 2021. She sees design as an art form, shaping exceptional products that seamlessly blend creativity and functionality.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/4bf1-400o400o1-ne6zrHPgJwZa3qp6qBPLGU.jpg</t>
+  </si>
+  <si>
+    <t>Ordering Coffee with Firebase AI</t>
+  </si>
+  <si>
+    <t>Check out my video submission: https://youtu.be/aW17mTF45yc
+ The presentation is not THE final yet, but it shows all the core idea, structure, and mood.
+ https://docs.google.com/presentation/d/1WRWVDhyplhf2odAEqYfv6whKdNIRipwwK-gf3Hn4sOo/edit?usp=sharing
+ I’m an Android Tech Lead at Dodo Brands, the fastest-growing QSR franchise company, operating internationally with Dodo Pizza and Drinkit coffee shops, including in the UAE.
+ My talk is called “Ordering Coffee with Firebase AI”, and it’s about a real case of bootstrapping AI assistants with Firebase AI Logic.
+ I’m working on a coffee shop chain app called Drinkit. Our menu is huge: you can customize drinks with or without milk, change ice, add syrups, literally millions of combinations. Too big for a static UI. So we thought: why not let AI guide the user? What if you could just say: “It’s hot today, give me something refreshing”. And boom, the app recommends the perfect drink for you. That’s exactly what we’re building in Drinkit.
+ I believe this talk will be useful because it’s a real production case of applying Firebase AI, not just sandbox examples. Attendees will see how we combined speech-to-text, Firebase AI models, and function calls to handle a huge menu (2M+ token context!) and deliver an interactive, personalized ordering experience. Developers will walk away with inspiration, code examples, and practical lessons on how to quickly bootstrap AI features in their own apps.</t>
+  </si>
+  <si>
+    <t>Max Kachinkin</t>
+  </si>
+  <si>
+    <t>maxkachinkin@gmail.com</t>
+  </si>
+  <si>
+    <t>1f2ba26b-921a-4b3a-ba24-1e8208f935b8</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Kachinkin</t>
+  </si>
+  <si>
+    <t>Android Tech Lead, Dodo Brands</t>
+  </si>
+  <si>
+    <t>Android Tech Lead, Dodo Brands
+ I have over 10 years of experience in Android development and currently work as an Android Tech Lead at Dodo Brands. I led the development of Dodo Pizza (with 9 million MAU across 20 countries) and am now working on another project, Drinkit, a new digital coffee shop network by Dodo Brands.
+ - I run a Telegram channel on mobile development, "Mobile Fiction"
+ - I speak at conferences such as Mobius and Codefest.
+ - I write articles on platforms like Habr, Medium (ProAndroidDev, BetterProgramming), HackerNoon.
+ - I teach Android development in the Android Professional course at OTUS.
+ - I created an Android Architecture course for GeekBrains Online School.
+ - I participate in the program committee for the Android Podlodka Crew conference.
+ - I also engage in various community activities, such as conducting an open interview, DevZen podcast.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/2b33-400o400o1-NAvjTdoBPX4kkGbQGnntqb.jpg</t>
+  </si>
+  <si>
+    <t>Actually optimizing your RAG with Gemini</t>
+  </si>
+  <si>
+    <t>Let's talk about making retrieval-augmented generation systems work better, faster, and cheaper by utilizing Gemini embedding models to do machine learning, semantic retrieval, and prompt optimizations</t>
+  </si>
+  <si>
+    <t>Armen Vardanyan</t>
+  </si>
+  <si>
+    <t>armenvardanyan95@gmail.com</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
-    <t>695c0a43-6758-4801-bb70-bb1e447b4df2</t>
-  </si>
-  <si>
-    <t>Seda</t>
-  </si>
-  <si>
-    <t>Sahakyan</t>
-  </si>
-  <si>
-    <t>Product Designer, iGameMedia</t>
-  </si>
-  <si>
-    <t>Seda, a product designer crafting digital experiences since 2021. She sees design as an art form, shaping exceptional products that seamlessly blend creativity and functionality.</t>
-  </si>
-  <si>
-    <t>https://sessionize.com/image/4bf1-400o400o1-ne6zrHPgJwZa3qp6qBPLGU.jpg</t>
-  </si>
-  <si>
-    <t>Ordering Coffee with Firebase AI</t>
-  </si>
-  <si>
-    <t>Check out my video submission: https://youtu.be/aW17mTF45yc
-The presentation is not THE final yet, but it shows all the core idea, structure, and mood.
-https://docs.google.com/presentation/d/1WRWVDhyplhf2odAEqYfv6whKdNIRipwwK-gf3Hn4sOo/edit?usp=sharing
-I’m an Android Tech Lead at Dodo Brands, the fastest-growing QSR franchise company, operating internationally with Dodo Pizza and Drinkit coffee shops, including in the UAE.
-My talk is called “Ordering Coffee with Firebase AI”, and it’s about a real case of bootstrapping AI assistants with Firebase AI Logic.
-I’m working on a coffee shop chain app called Drinkit. Our menu is huge: you can customize drinks with or without milk, change ice, add syrups, literally millions of combinations. Too big for a static UI. So we thought: why not let AI guide the user? What if you could just say: “It’s hot today, give me something refreshing”. And boom, the app recommends the perfect drink for you. That’s exactly what we’re building in Drinkit.
-I believe this talk will be useful because it’s a real production case of applying Firebase AI, not just sandbox examples. Attendees will see how we combined speech-to-text, Firebase AI models, and function calls to handle a huge menu (2M+ token context!) and deliver an interactive, personalized ordering experience. Developers will walk away with inspiration, code examples, and practical lessons on how to quickly bootstrap AI features in their own apps.</t>
-  </si>
-  <si>
-    <t>Max Kachinkin</t>
-  </si>
-  <si>
-    <t>maxkachinkin@gmail.com</t>
-  </si>
-  <si>
-    <t>Room 1</t>
-  </si>
-  <si>
-    <t>1f2ba26b-921a-4b3a-ba24-1e8208f935b8</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Kachinkin</t>
-  </si>
-  <si>
-    <t>Android Tech Lead, Dodo Brands</t>
-  </si>
-  <si>
-    <t>Android Tech Lead, Dodo Brands
-I have over 10 years of experience in Android development and currently work as an Android Tech Lead at Dodo Brands. I led the development of Dodo Pizza (with 9 million MAU across 20 countries) and am now working on another project, Drinkit, a new digital coffee shop network by Dodo Brands.
-- I run a Telegram channel on mobile development, "Mobile Fiction"
-- I speak at conferences such as Mobius and Codefest.
-- I write articles on platforms like Habr, Medium (ProAndroidDev, BetterProgramming), HackerNoon.
-- I teach Android development in the Android Professional course at OTUS.
-- I created an Android Architecture course for GeekBrains Online School.
-- I participate in the program committee for the Android Podlodka Crew conference.
-- I also engage in various community activities, such as conducting an open interview, DevZen podcast.</t>
-  </si>
-  <si>
-    <t>https://sessionize.com/image/2b33-400o400o1-NAvjTdoBPX4kkGbQGnntqb.jpg</t>
+    <t>b3a2e3aa-4e66-41dc-83a9-8209803c914f</t>
+  </si>
+  <si>
+    <t>Armen</t>
+  </si>
+  <si>
+    <t>Vardanyan</t>
+  </si>
+  <si>
+    <t>Google Developer Expert for Angular, Front-End Team Lead</t>
+  </si>
+  <si>
+    <t>Front End Team Lead working with Angular for 6+ years, GDE for Angular, technical writer, mentor, speaker.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/ccc2-400o400o1-futBYou8hfX59EBdSrY52r.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d MMM yyyy HH:mm AM/PM"/>
+    <numFmt numFmtId="165" formatCode="d mmm yyyy h:mm am/pm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -206,13 +242,19 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -242,7 +284,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border/>
     <border>
       <left/>
@@ -250,22 +292,46 @@
       <top/>
       <bottom/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF9A9A9A"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF9A9A9A"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF9A9A9A"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9A9A9A"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -482,7 +548,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="8.71"/>
+    <col customWidth="1" min="2" max="2" width="89.0"/>
+    <col customWidth="1" min="3" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -548,7 +616,7 @@
       <c r="A2" s="4">
         <v>1062404.0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -560,15 +628,23 @@
       <c r="E2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="6">
-        <v>45953.493480324076</v>
-      </c>
-      <c r="G2" s="6">
-        <v>45953.50132827546</v>
+      <c r="F2" s="5">
+        <v>45953.493055555555</v>
+      </c>
+      <c r="G2" s="5">
+        <v>45953.50069444445</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="I2" s="6">
+        <v>46011.4375</v>
+      </c>
+      <c r="J2" s="4">
+        <v>120.0</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
       <c r="M2" s="4" t="s">
         <v>24</v>
       </c>
@@ -587,7 +663,7 @@
       <c r="R2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -607,15 +683,23 @@
       <c r="E3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="6">
-        <v>45957.70936790509</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="5">
+        <v>45957.709027777775</v>
+      </c>
+      <c r="G3" s="6">
+        <v>45958.175</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="I3" s="6">
+        <v>46011.4375</v>
+      </c>
+      <c r="J3" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
       <c r="M3" s="4" t="s">
         <v>35</v>
       </c>
@@ -634,7 +718,7 @@
       <c r="R3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="8" t="s">
         <v>40</v>
       </c>
     </row>
@@ -654,41 +738,98 @@
       <c r="E4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="6">
-        <v>45951.567294988425</v>
-      </c>
-      <c r="G4" s="6">
-        <v>45951.57514247685</v>
+      <c r="F4" s="5">
+        <v>45951.566666666666</v>
+      </c>
+      <c r="G4" s="5">
+        <v>45951.575</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="6">
-        <v>46011.375</v>
+        <v>34</v>
+      </c>
+      <c r="I4" s="5">
+        <v>46011.458333333336</v>
       </c>
       <c r="J4" s="4">
         <v>30.0</v>
       </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
       <c r="M4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>44</v>
       </c>
       <c r="Q4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="R4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="S4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="S4" s="4" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="4">
+        <v>1066127.0</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>51</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="6">
+        <v>45959.54722222222</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="6">
+        <v>46011.479166666664</v>
+      </c>
+      <c r="J5" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -1672,9 +1813,15 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="S2"/>
+    <hyperlink r:id="rId2" ref="S3"/>
+    <hyperlink r:id="rId3" ref="S4"/>
+    <hyperlink r:id="rId4" ref="S5"/>
+  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add new session and speaker details for Kirill Cherniavski and Dr Roushanak Rahmat
</commit_message>
<xml_diff>
--- a/public/devfest-armenia-2025-flattened-sessions.xlsx
+++ b/public/devfest-armenia-2025-flattened-sessions.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="3U3RRnnZISOg2CxmXwC8bfIO1FZhGfQOys4rEufgizc="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="sr00md8a71N4E0xGXvGDb5QJFUGrVrH70E/vdKEcCP4="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="92">
   <si>
     <t>Session Id</t>
   </si>
@@ -73,6 +73,80 @@
   </si>
   <si>
     <t>Profile Picture</t>
+  </si>
+  <si>
+    <t>Go Beyond Models: Why AI Needs a Fast Backend</t>
+  </si>
+  <si>
+    <t>Al models get all the attention, but real-world systems live and die by their backend. Go has quietly become a favorite for building the infrastructure behind Al - from API gateways and streaming responses to agent runtimes and data pipelines.
+ In this talk, I'll show why Go's simplicity, concurrency model, and reliability make it great for Al backends. We'll look at examples of how Go powers fast, scalable services around large language models, and what lessons Go engineers can borrow from the Al world (and vice versa).</t>
+  </si>
+  <si>
+    <t>Kirill Cherniavski</t>
+  </si>
+  <si>
+    <t>g4s8.public@gmail.com</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>bee2fa27-358d-4a18-9796-938a9229ca00</t>
+  </si>
+  <si>
+    <t>Kirill</t>
+  </si>
+  <si>
+    <t>Cherniavski</t>
+  </si>
+  <si>
+    <t>Just a software engineer</t>
+  </si>
+  <si>
+    <t>12 years of experience, moved from java to go 6 years ago. Ex principal engineer in Huawei (cloud department). Building high-load apps and distributed systems.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/0f4f-400o400o1-325zV56GBzG8KTAwZDjWyK.jpg</t>
+  </si>
+  <si>
+    <t>Agent-to-Agent (A2A) Protocol: A Deep Dive into Google’s Client-Server Model</t>
+  </si>
+  <si>
+    <t>This session takes a deep dive into Google’s Agent-to-Agent (A2A) protocol, focusing on its client–server model and the Purchasing Concierge example. We’ll explore how A2A enables autonomous agents to communicate, delegate tasks, and coordinate across distributed systems, moving beyond simple tool invocation toward true agent ecosystems. Through real-world workflows, you’ll see how agents discover each other, exchange structured messages, and orchestrate multi-step interactions. By the end, you’ll understand the architectural principles behind A2A and how to apply them to build scalable, collaborative AI solutions.</t>
+  </si>
+  <si>
+    <t>Dr Roushanak Rahmat</t>
+  </si>
+  <si>
+    <t>roushanakrahmat@gmail.com</t>
+  </si>
+  <si>
+    <t>085f6e1b-c573-4ea3-af24-dd5ab8a9d7be</t>
+  </si>
+  <si>
+    <t>Dr Roushanak</t>
+  </si>
+  <si>
+    <t>Rahmat</t>
+  </si>
+  <si>
+    <t>Lead Data Scientist</t>
+  </si>
+  <si>
+    <t>I’m Dr Roushanak Rahmat, a Lead AI Architect and Strategist, Google Developer Expert (AI &amp; Cloud), and recognised as one of the Top 100 Women in Tech (2025). With a PhD in Artificial Intelligence and over a decade of experience, I specialise in architecting and delivering enterprise-scale Generative AI, Agentic AI, and Deep Learning solutions that drive innovation across healthcare, finance, and energy.
+ At IBM Consulting, I design and implement AI and GenAI strategies, building LLM-powered systems, RAG pipelines, and multi-agent frameworks that enhance enterprise workflows, decision-making, and long-term scalability. So far, I have contributed to projects for clients including KPMG, NHS, Scottish Power, Coca-Cola, and Lloyds Banking, helping them explore responsible and scalable adoption of AI technologies.
+ Previously at Elekta, I led AI innovation projects that advanced radiotherapy through multimodal imaging and deep learning, resulting in multiple US patents in medical AI. My research and applied work have directly contributed to improving patient outcomes in oncology and clinical imaging.
+ I am also a Google Women Techmakers Ambassador, public speaker, and active contributor to the AI community through talks, technical Medium blogs, YouTube, and open-source projects. Beyond technical expertise, I am passionate about bridging the gap between cutting-edge AI research and real-world business impact, while mentoring and inspiring the next generation of AI leaders.
+ 🔑 Highlights:
+ ✅ Top 100 Women in Tech (2025) – WeAreTechWomen &amp; UN UK Women Delegate
+ ✅ US Patent Inventor in medical AI (advanced imaging &amp; radiotherapy)
+ ✅ Google Developer Expert (AI &amp; Cloud)
+ ✅ Experienced in cloud-native AI (GCP, AWS, Azure, IBM watsonx) and modern ML stacks (LangChain, PyTorch, TensorFlow, JAX)
+ ✅ Associate Professor shaping the next generation of AI talent
+ Explore my portfolio: roushanakrahmat.github.io</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/ba90-400o400o1-fzqoL9qQ9sABBDWiSraopL.png</t>
   </si>
   <si>
     <t>Agent Development Kit Deep Dive [WORKSHOP]</t>
@@ -199,9 +273,6 @@
     <t>armenvardanyan95@gmail.com</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>b3a2e3aa-4e66-41dc-83a9-8209803c914f</t>
   </si>
   <si>
@@ -260,7 +331,7 @@
     <numFmt numFmtId="164" formatCode="d MMM yyyy HH:mm AM/PM"/>
     <numFmt numFmtId="165" formatCode="d mmm yyyy h:mm am/pm"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -282,6 +353,16 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <u/>
@@ -342,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -355,14 +436,29 @@
     <xf borderId="2" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,7 +742,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4">
-        <v>1062404.0</v>
+        <v>1069411.0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>19</v>
@@ -661,22 +757,16 @@
         <v>22</v>
       </c>
       <c r="F2" s="5">
-        <v>45953.493055555555</v>
-      </c>
-      <c r="G2" s="5">
-        <v>45953.50069444445</v>
-      </c>
-      <c r="H2" s="4" t="s">
+        <v>45963.40416666667</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="6">
-        <v>46011.4375</v>
-      </c>
-      <c r="J2" s="4">
-        <v>120.0</v>
-      </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
       <c r="M2" s="4" t="s">
         <v>24</v>
       </c>
@@ -701,7 +791,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4">
-        <v>1064706.0</v>
+        <v>1069557.0</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>30</v>
@@ -716,211 +806,313 @@
         <v>33</v>
       </c>
       <c r="F3" s="5">
-        <v>45957.709027777775</v>
-      </c>
-      <c r="G3" s="6">
-        <v>45958.175</v>
-      </c>
-      <c r="H3" s="4" t="s">
+        <v>45963.40416666667</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="6">
-        <v>46011.4375</v>
-      </c>
-      <c r="J3" s="4">
-        <v>30.0</v>
-      </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="Q3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4">
-        <v>1060533.0</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="9">
+        <v>1062404.0</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="10">
+        <v>45953.493055555555</v>
+      </c>
+      <c r="G4" s="10">
+        <v>45953.50069444445</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="5">
-        <v>45951.566666666666</v>
-      </c>
-      <c r="G4" s="5">
-        <v>45951.575</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="5">
-        <v>46011.458333333336</v>
-      </c>
-      <c r="J4" s="4">
-        <v>30.0</v>
-      </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="4" t="s">
+      <c r="I4" s="11">
+        <v>46011.4375</v>
+      </c>
+      <c r="J4" s="9">
+        <v>120.0</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q4" s="4" t="s">
+      <c r="P4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q4" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="S4" s="13" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4">
-        <v>1066127.0</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="9">
+        <v>1064706.0</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="6">
-        <v>45959.54722222222</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="10">
+        <v>45957.709027777775</v>
+      </c>
+      <c r="G5" s="11">
+        <v>45958.175</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="6">
-        <v>46011.479166666664</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="I5" s="11">
+        <v>46011.4375</v>
+      </c>
+      <c r="J5" s="9">
         <v>30.0</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="4" t="s">
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="Q5" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="S5" s="8" t="s">
+      <c r="S5" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4">
+      <c r="A6" s="9">
+        <v>1060533.0</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="10">
+        <v>45951.566666666666</v>
+      </c>
+      <c r="G6" s="10">
+        <v>45951.575</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="10">
+        <v>46011.458333333336</v>
+      </c>
+      <c r="J6" s="9">
+        <v>30.0</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="S6" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="9">
+        <v>1066127.0</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="11">
+        <v>45959.54722222222</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="11">
+        <v>46011.479166666664</v>
+      </c>
+      <c r="J7" s="9">
+        <v>30.0</v>
+      </c>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="S7" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="9">
         <v>1061298.0</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="B8" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="11">
         <v>45960.46875</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="6">
+      <c r="I8" s="11">
         <v>46011.5</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J8" s="9">
         <v>10.0</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="S6" s="8" t="s">
-        <v>71</v>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="S8" s="13" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
     <row r="25" ht="15.75" customHeight="1"/>
@@ -1899,6 +2091,8 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="S2"/>
@@ -1906,10 +2100,12 @@
     <hyperlink r:id="rId3" ref="S4"/>
     <hyperlink r:id="rId4" ref="S5"/>
     <hyperlink r:id="rId5" ref="S6"/>
+    <hyperlink r:id="rId6" ref="S7"/>
+    <hyperlink r:id="rId7" ref="S8"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update speaker details for Dr Roushanak Rahmat to include current position and affiliations
</commit_message>
<xml_diff>
--- a/public/devfest-armenia-2025-flattened-sessions.xlsx
+++ b/public/devfest-armenia-2025-flattened-sessions.xlsx
@@ -130,20 +130,14 @@
     <t>Rahmat</t>
   </si>
   <si>
-    <t>Lead Data Scientist</t>
-  </si>
-  <si>
-    <t>I’m Dr Roushanak Rahmat, a Lead AI Architect and Strategist, Google Developer Expert (AI &amp; Cloud), and recognised as one of the Top 100 Women in Tech (2025). With a PhD in Artificial Intelligence and over a decade of experience, I specialise in architecting and delivering enterprise-scale Generative AI, Agentic AI, and Deep Learning solutions that drive innovation across healthcare, finance, and energy.
- At IBM Consulting, I design and implement AI and GenAI strategies, building LLM-powered systems, RAG pipelines, and multi-agent frameworks that enhance enterprise workflows, decision-making, and long-term scalability. So far, I have contributed to projects for clients including KPMG, NHS, Scottish Power, Coca-Cola, and Lloyds Banking, helping them explore responsible and scalable adoption of AI technologies.
- Previously at Elekta, I led AI innovation projects that advanced radiotherapy through multimodal imaging and deep learning, resulting in multiple US patents in medical AI. My research and applied work have directly contributed to improving patient outcomes in oncology and clinical imaging.
- I am also a Google Women Techmakers Ambassador, public speaker, and active contributor to the AI community through talks, technical Medium blogs, YouTube, and open-source projects. Beyond technical expertise, I am passionate about bridging the gap between cutting-edge AI research and real-world business impact, while mentoring and inspiring the next generation of AI leaders.
- 🔑 Highlights:
- ✅ Top 100 Women in Tech (2025) – WeAreTechWomen &amp; UN UK Women Delegate
- ✅ US Patent Inventor in medical AI (advanced imaging &amp; radiotherapy)
- ✅ Google Developer Expert (AI &amp; Cloud)
- ✅ Experienced in cloud-native AI (GCP, AWS, Azure, IBM watsonx) and modern ML stacks (LangChain, PyTorch, TensorFlow, JAX)
- ✅ Associate Professor shaping the next generation of AI talent
- Explore my portfolio: roushanakrahmat.github.io</t>
+    <t>Lead Data Scientist, IBM, Google Developer Expert (AI &amp; Cloud)</t>
+  </si>
+  <si>
+    <t>Dr Roushanak Rahmat is a Google Developer Expert and seasoned AI Strategy Leader with a PhD in Artificial Intelligence, specializing in computer vision and image processing. With over a decade of hands-on experience in designing, delivering, and scaling AI and Generative AI (GenAI) solutions, she has partnered with leading organizations including IBM, the NHS, Elekta, Coca-Cola, Lloyds, and Scottish Power to transform complex challenges into measurable business outcomes.
+Currently serving as a Lead Data Scientist at IBM Consulting, Roushanak leads the development and deployment of AI and GenAI strategies across sectors such as healthcare, finance, and energy. Her work focuses on translating cutting-edge research into real-world applications, ensuring that innovation remains both technically sound and strategically aligned with business goals.
+Prior to IBM, she played a pivotal role at Elekta, a global leader in cancer treatment solutions. There, she led innovation projects harnessing deep learning and multimodal medical imaging to enhance radiotherapy outcomes. Her technical toolkit includes Python, PyTorch, TensorFlow, Keras, and JAX, with domain expertise in working with MRI, CT, and CBCT imaging data, as well as large-scale data pipelines and analytics platforms.
+Beyond her technical contributions, Roushanak is a dedicated advocate for ethical AI, inclusive innovation, and knowledge sharing. She serves as a Women Techmakers ambassador, where she champions diversity in tech and mentors emerging talent in AI and data science. Her passion for democratizing AI knowledge is evident in her active online presence—sharing insights through Medium articles, open-source contributions, and educational content on YouTube.
+Known for her ability to bridge the gap between deeply technical teams and executive stakeholders, Roushanak excels at aligning AI initiatives with strategic business objectives. Whether speaking at conferences, mentoring early-career professionals, or advising C-suite leaders, she brings clarity, purpose, and impact to every conversation around AI.</t>
   </si>
   <si>
     <t>https://sessionize.com/image/ba90-400o400o1-fzqoL9qQ9sABBDWiSraopL.png</t>
@@ -678,7 +672,9 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="8.71"/>
     <col customWidth="1" min="2" max="2" width="89.0"/>
-    <col customWidth="1" min="3" max="26" width="8.71"/>
+    <col customWidth="1" min="3" max="16" width="8.71"/>
+    <col customWidth="1" min="17" max="17" width="48.14"/>
+    <col customWidth="1" min="18" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Add new sessions and speakers; update speaker details and add Google for Developers logo
</commit_message>
<xml_diff>
--- a/public/devfest-armenia-2025-flattened-sessions.xlsx
+++ b/public/devfest-armenia-2025-flattened-sessions.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="sr00md8a71N4E0xGXvGDb5QJFUGrVrH70E/vdKEcCP4="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="ELyHtuFYp6WvJEyXNJTQaQsro16tELuKXqo8m3ejQhY="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="142">
   <si>
     <t>Session Id</t>
   </si>
@@ -75,38 +75,147 @@
     <t>Profile Picture</t>
   </si>
   <si>
-    <t>Go Beyond Models: Why AI Needs a Fast Backend</t>
-  </si>
-  <si>
-    <t>Al models get all the attention, but real-world systems live and die by their backend. Go has quietly become a favorite for building the infrastructure behind Al - from API gateways and streaming responses to agent runtimes and data pipelines.
- In this talk, I'll show why Go's simplicity, concurrency model, and reliability make it great for Al backends. We'll look at examples of how Go powers fast, scalable services around large language models, and what lessons Go engineers can borrow from the Al world (and vice versa).</t>
-  </si>
-  <si>
-    <t>Kirill Cherniavski</t>
-  </si>
-  <si>
-    <t>g4s8.public@gmail.com</t>
+    <t>Simple Emotional Intelligence Skills [WORKSHOP]</t>
+  </si>
+  <si>
+    <t>As AI gets smarter — coding, making presentations, even writing texts (maybe this one too!) — let’s invest in what can’t be delegated to machines: emotional intelligence.
+ This hands-on workshop is built around simple, practical exercises that strengthen key soft skills — listening, collaboration, and learning — with a special focus on how to give advice the right way.
+ Expect minimal theory, maximum practice, and a few unexpected stories along the way.
+ Come with an open mind and be ready to take part.
+ At the very least, it’ll be fun — and at best, surprisingly useful. 🌿</t>
+  </si>
+  <si>
+    <t>Natasha Arefyeva</t>
+  </si>
+  <si>
+    <t>narefyeva.coach@gmail.com</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>bee2fa27-358d-4a18-9796-938a9229ca00</t>
-  </si>
-  <si>
-    <t>Kirill</t>
-  </si>
-  <si>
-    <t>Cherniavski</t>
-  </si>
-  <si>
-    <t>Just a software engineer</t>
-  </si>
-  <si>
-    <t>12 years of experience, moved from java to go 6 years ago. Ex principal engineer in Huawei (cloud department). Building high-load apps and distributed systems.</t>
-  </si>
-  <si>
-    <t>https://sessionize.com/image/0f4f-400o400o1-325zV56GBzG8KTAwZDjWyK.jpg</t>
+    <t>fcd40625-d41f-45f8-8b4b-fc510bb96d07</t>
+  </si>
+  <si>
+    <t>Natasha</t>
+  </si>
+  <si>
+    <t>Arefyeva</t>
+  </si>
+  <si>
+    <t>ACC ICF Certified Coach, 15+ years in IT</t>
+  </si>
+  <si>
+    <t>Natasha Arefyeva has spent over 15 years in tech — from developer to Chief Product Officer.
+ Now an ACC ICF coach (Erickson Coaching International, Canada) and team coach, she helps people and teams reconnect with clarity, trust, and purpose.
+ Her work focuses on building honest, open communication and processes that make teams stronger from the inside out.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/7f26-400o400o1-MDc9fdZAHv4bp3BpAM19fh.jpg</t>
+  </si>
+  <si>
+    <t>Beyond the Prompt: An Anatomy of an AI-powered Game using Agent Development Kit</t>
+  </si>
+  <si>
+    <t>LLMs have opened up a world of possibilities, but turning them into a truly useful, AI-driven application presents a unique set of challenges. Brought to you by a professional game maker, in this talk, we’ll use an AI-powered game as a practical example to explore these real-world hurdles and see how Agent Development Kit can help solve them.
+ You’ll learn how to:
+ Design an application using an agent-based architecture, with the responsible use of AI in mind.
+ Use input and output schemas to exchange structured data between agents and the front-end.
+ Manage game state using session state.
+ Control the game flow with a custom orchestrator agent.</t>
+  </si>
+  <si>
+    <t>Yoyu Li</t>
+  </si>
+  <si>
+    <t>yoyu777@gmail.com</t>
+  </si>
+  <si>
+    <t>Hall A</t>
+  </si>
+  <si>
+    <t>7fd4159e-a3e4-4ebf-93d9-62c78f7e8323</t>
+  </si>
+  <si>
+    <t>Yoyu</t>
+  </si>
+  <si>
+    <t>Li</t>
+  </si>
+  <si>
+    <t>Igniting Creativity with Technology</t>
+  </si>
+  <si>
+    <t>Yoyu is a creative technology advisor at Infinite Whys. She has worked in a wide range of capacities throughout her career - product designer, game producer, product manager, startup CTO and technology consultant.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/845b-400o400o1-TbTE3pLpPy7QH8G2YiZzoj.jpg</t>
+  </si>
+  <si>
+    <t>Accelerate AI with Cloud Run: deploy a MCP server on Cloud Run [WORKSHOP]</t>
+  </si>
+  <si>
+    <t>The workshop delves into the architectural pattern for deploying a secure and scalable MCP server (a standard protocol that enables AI models to connect with and utilize external tools and data sources) on GCP's renowned Cloud Run and covers Cloud Run GPU capabilities.</t>
+  </si>
+  <si>
+    <t>Rohan Singh</t>
+  </si>
+  <si>
+    <t>rohandash1998@gmail.com</t>
+  </si>
+  <si>
+    <t>Wokshop</t>
+  </si>
+  <si>
+    <t>9d696680-4fd0-4fa5-8d96-f93515a3910c</t>
+  </si>
+  <si>
+    <t>Rohan</t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>Senior Cloud Platform Engineer at SADA, an Insight Company | Google Developer Expert - Google Cloud | GDG Yerevan - Co Organizer</t>
+  </si>
+  <si>
+    <t>A dynamic Indian cloud guy and avid community lover with a devotion to motorcycling working and living in Armenia.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/8127-400o400o1-G6DGgUfqS9qdu6SEvW7XwU.jpg</t>
+  </si>
+  <si>
+    <t>Beyond Next.js: TanStack Start and the Future of Full-Stack React Development</t>
+  </si>
+  <si>
+    <t>Next.js has dominated the React ecosystem for quite a while, but TanStack Start is making developers reconsider. Is it a genuine replacement or a specialized alternative?
+ We'll compare the architectural philosophies – server-first vs. client-first, all-in-one vs. composable – and break down the real trade-offs in routing, data fetching, and ecosystem maturity. Through technical analysis and candid perspective, we'll examine when to reach for TanStack Start, when Next.js remains the better choice, and what this evolution means for full-stack React development.
+ Expect a balanced view grounded in actual experience: what works, what doesn't, and what the community is building with these frameworks.</t>
+  </si>
+  <si>
+    <t>Viktoriia Akhmatova</t>
+  </si>
+  <si>
+    <t>toriatovawebdev@gmail.com</t>
+  </si>
+  <si>
+    <t>4f4a4f3f-0751-41f1-b1ad-d4edd8cd09c5</t>
+  </si>
+  <si>
+    <t>Viktoriia</t>
+  </si>
+  <si>
+    <t>Akhmatova</t>
+  </si>
+  <si>
+    <t>Jack of all trades</t>
+  </si>
+  <si>
+    <t>Full-stack developer developer with 5+ years of experience building modern web applications. My main tools are TypeScript, React, and Next.js, which I use across the stack – from frontend logic to backend APIs and production setups.
+ I love exploring new tech and experiment with it :3</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/37eb-400o400o1-VMZhK1e9g59mZBcH2MZnCK.jpg</t>
   </si>
   <si>
     <t>Agent-to-Agent (A2A) Protocol: A Deep Dive into Google’s Client-Server Model</t>
@@ -143,37 +252,95 @@
     <t>https://sessionize.com/image/ba90-400o400o1-fzqoL9qQ9sABBDWiSraopL.png</t>
   </si>
   <si>
-    <t>Agent Development Kit Deep Dive [WORKSHOP]</t>
-  </si>
-  <si>
-    <t>From Initialization to Ideation to Prompting to Deployment. All of these and the intermediate steps will be covered in the creation of your own Agent application. We all know about AI, but this is much more than that, it is making sure the AI is deployed and available in the most consistent way possible with all the requirements for application development including version control, testing and scaling being covered. You will be given credits to follow along on the workshop.</t>
-  </si>
-  <si>
-    <t>Ankur Roy</t>
-  </si>
-  <si>
-    <t>ankur.roy@onlinepartner.se</t>
-  </si>
-  <si>
-    <t>Wokshop</t>
-  </si>
-  <si>
-    <t>8ca460b2-bb7b-4e0a-bc41-7a7ddcb2dda3</t>
-  </si>
-  <si>
-    <t>Ankur</t>
-  </si>
-  <si>
-    <t>Roy</t>
-  </si>
-  <si>
-    <t>Solutions Architect at Online Partner AB | Google Developer Expert in Cloud</t>
-  </si>
-  <si>
-    <t>I am a Solutions Architect at Online Partner AB and a Cloud GDE. I have worked on several projects involving Google Cloud services and Google Workspace along with multiple other technology stacks and platforms.</t>
-  </si>
-  <si>
-    <t>https://sessionize.com/image/7b5c-400o400o1-LM8dCULuUeHrEhCsuRY34o.jpg</t>
+    <t>Go Beyond Models: Why AI Needs a Fast Backend</t>
+  </si>
+  <si>
+    <t>Al models get all the attention, but real-world systems live and die by their backend. Go has quietly become a favorite for building the infrastructure behind Al - from API gateways and streaming responses to agent runtimes and data pipelines.
+ In this talk, I'll show why Go's simplicity, concurrency model, and reliability make it great for Al backends. We'll look at examples of how Go powers fast, scalable services around large language models, and what lessons Go engineers can borrow from the Al world (and vice versa).</t>
+  </si>
+  <si>
+    <t>Kirill Cherniavski</t>
+  </si>
+  <si>
+    <t>g4s8.public@gmail.com</t>
+  </si>
+  <si>
+    <t>bee2fa27-358d-4a18-9796-938a9229ca00</t>
+  </si>
+  <si>
+    <t>Kirill</t>
+  </si>
+  <si>
+    <t>Cherniavski</t>
+  </si>
+  <si>
+    <t>Just a software engineer</t>
+  </si>
+  <si>
+    <t>12 years of experience, moved from java to go 6 years ago. Ex principal engineer in Huawei (cloud department). Building high-load apps and distributed systems.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/0f4f-400o400o1-325zV56GBzG8KTAwZDjWyK.jpg</t>
+  </si>
+  <si>
+    <t>Engineering Leadership for Distributed Teams: Balancing Code, People, and Culture</t>
+  </si>
+  <si>
+    <t>Leading a distributed engineering team is more than managing tasks across time zones — it’s about building trust, maintaining technical excellence, and keeping a shared culture alive. In this talk I will share lessons from managing multinational teams while staying hands-on with code. You’ll learn practical approaches to balancing leadership and technical work, fostering innovation, and scaling remote collaboration without losing team spirit.</t>
+  </si>
+  <si>
+    <t>Davit Siradeghyan</t>
+  </si>
+  <si>
+    <t>davitsiradeghyan@gmail.com</t>
+  </si>
+  <si>
+    <t>5657af52-88d4-442d-b10b-809459437af5</t>
+  </si>
+  <si>
+    <t>Davit</t>
+  </si>
+  <si>
+    <t>Siradeghyan</t>
+  </si>
+  <si>
+    <t>Engineering Manager at Softr</t>
+  </si>
+  <si>
+    <t>My name is Davit, and I’m currently an Engineering Manager at Softr. I bring over 15 years of experience across US, Canadian, and European companies, both startups and enterprises. My career started as a C++ developer working in electronic design automation and high-performance trading systems (6+ years, mostly at Questrade). Later, I transitioned into iOS development, contributing to companies such as Workfront (acquired by Adobe), Zero (now Hercules.ai), and Disqo for another 6+ years. For the past few years, I’ve been leading engineering at Softr, while still remaining hands-on in coding (around 70% of my time, primarily in Java).</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/cb44-400o400o1-ndd8tsfsG4cPgo6uJZeZL9.jpg</t>
+  </si>
+  <si>
+    <t>Actually optimizing your RAG with Gemini</t>
+  </si>
+  <si>
+    <t>Let's talk about making retrieval-augmented generation systems work better, faster, and cheaper by utilizing Gemini embedding models to do machine learning, semantic retrieval, and prompt optimizations</t>
+  </si>
+  <si>
+    <t>Armen Vardanyan</t>
+  </si>
+  <si>
+    <t>armenvardanyan95@gmail.com</t>
+  </si>
+  <si>
+    <t>b3a2e3aa-4e66-41dc-83a9-8209803c914f</t>
+  </si>
+  <si>
+    <t>Armen</t>
+  </si>
+  <si>
+    <t>Vardanyan</t>
+  </si>
+  <si>
+    <t>Google Developer Expert for Angular, Front-End Team Lead</t>
+  </si>
+  <si>
+    <t>Front End Team Lead working with Angular for 6+ years, GDE for Angular, technical writer, mentor, speaker.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/ccc2-400o400o1-futBYou8hfX59EBdSrY52r.jpg</t>
   </si>
   <si>
     <t>How Far Should You Go with AI? Automating Product Creation While Keeping the Balance</t>
@@ -190,9 +357,6 @@
     <t>seda.design05@gmail.com</t>
   </si>
   <si>
-    <t>Hall A</t>
-  </si>
-  <si>
     <t>695c0a43-6758-4801-bb70-bb1e447b4df2</t>
   </si>
   <si>
@@ -209,6 +373,68 @@
   </si>
   <si>
     <t>https://sessionize.com/image/4bf1-400o400o1-ne6zrHPgJwZa3qp6qBPLGU.jpg</t>
+  </si>
+  <si>
+    <t>Agent Development Kit Deep Dive [WORKSHOP]</t>
+  </si>
+  <si>
+    <t>From Initialization to Ideation to Prompting to Deployment. All of these and the intermediate steps will be covered in the creation of your own Agent application. We all know about AI, but this is much more than that, it is making sure the AI is deployed and available in the most consistent way possible with all the requirements for application development including version control, testing and scaling being covered. You will be given credits to follow along on the workshop.</t>
+  </si>
+  <si>
+    <t>Ankur Roy</t>
+  </si>
+  <si>
+    <t>ankur.roy@onlinepartner.se</t>
+  </si>
+  <si>
+    <t>8ca460b2-bb7b-4e0a-bc41-7a7ddcb2dda3</t>
+  </si>
+  <si>
+    <t>Ankur</t>
+  </si>
+  <si>
+    <t>Roy</t>
+  </si>
+  <si>
+    <t>Solutions Architect at Online Partner AB | Google Developer Expert in Cloud</t>
+  </si>
+  <si>
+    <t>I am a Solutions Architect at Online Partner AB and a Cloud GDE. I have worked on several projects involving Google Cloud services and Google Workspace along with multiple other technology stacks and platforms.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/7b5c-400o400o1-LM8dCULuUeHrEhCsuRY34o.jpg</t>
+  </si>
+  <si>
+    <t>OAuth supply-chain risks: How to mitigate them, and how not to become them</t>
+  </si>
+  <si>
+    <t>A lightning session about Google APIs' OAuth permission scopes and their categories - from a security engineer's perspective. 
+ Topics include an introduction to supply chain risks, OAuth illicit consent attacks, 
+ The talk intends to be an awareness session for developers to request the least possible amount of permissions (and data) and for security engineers to audit their Google Workspace OAuth integrations.</t>
+  </si>
+  <si>
+    <t>Narek Babajanyan</t>
+  </si>
+  <si>
+    <t>narek_babajanyan@outlook.com</t>
+  </si>
+  <si>
+    <t>70d1cacf-57c0-4903-ab30-ef0faf6f1955</t>
+  </si>
+  <si>
+    <t>Narek</t>
+  </si>
+  <si>
+    <t>Babajanyan</t>
+  </si>
+  <si>
+    <t>Cybersecurity @ ServiceTitan | Armed Forces ex-officer</t>
+  </si>
+  <si>
+    <t>I am currently an Incident Response and Threat Prevention Engineer at ServiceTitan. Previously, I helped safeguard Armenia's critical infrastructure at the Information Systems Agency of Armenia.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/71f5-400o400o1-BVLaZdEqXxPwDdXZowmvfo.png</t>
   </si>
   <si>
     <t>Ordering Coffee with Firebase AI</t>
@@ -254,76 +480,14 @@
   <si>
     <t>https://sessionize.com/image/2b33-400o400o1-NAvjTdoBPX4kkGbQGnntqb.jpg</t>
   </si>
-  <si>
-    <t>Actually optimizing your RAG with Gemini</t>
-  </si>
-  <si>
-    <t>Let's talk about making retrieval-augmented generation systems work better, faster, and cheaper by utilizing Gemini embedding models to do machine learning, semantic retrieval, and prompt optimizations</t>
-  </si>
-  <si>
-    <t>Armen Vardanyan</t>
-  </si>
-  <si>
-    <t>armenvardanyan95@gmail.com</t>
-  </si>
-  <si>
-    <t>b3a2e3aa-4e66-41dc-83a9-8209803c914f</t>
-  </si>
-  <si>
-    <t>Armen</t>
-  </si>
-  <si>
-    <t>Vardanyan</t>
-  </si>
-  <si>
-    <t>Google Developer Expert for Angular, Front-End Team Lead</t>
-  </si>
-  <si>
-    <t>Front End Team Lead working with Angular for 6+ years, GDE for Angular, technical writer, mentor, speaker.</t>
-  </si>
-  <si>
-    <t>https://sessionize.com/image/ccc2-400o400o1-futBYou8hfX59EBdSrY52r.jpg</t>
-  </si>
-  <si>
-    <t>OAuth supply-chain risks: How to mitigate them, and how not to become them</t>
-  </si>
-  <si>
-    <t>A lightning session about Google APIs' OAuth permission scopes and their categories - from a security engineer's perspective. 
- Topics include an introduction to supply chain risks, OAuth illicit consent attacks, 
- The talk intends to be an awareness session for developers to request the least possible amount of permissions (and data) and for security engineers to audit their Google Workspace OAuth integrations.</t>
-  </si>
-  <si>
-    <t>Narek Babajanyan</t>
-  </si>
-  <si>
-    <t>narek_babajanyan@outlook.com</t>
-  </si>
-  <si>
-    <t>70d1cacf-57c0-4903-ab30-ef0faf6f1955</t>
-  </si>
-  <si>
-    <t>Narek</t>
-  </si>
-  <si>
-    <t>Babajanyan</t>
-  </si>
-  <si>
-    <t>Cybersecurity @ ServiceTitan | Armed Forces ex-officer</t>
-  </si>
-  <si>
-    <t>I am currently an Incident Response and Threat Prevention Engineer at ServiceTitan. Previously, I helped safeguard Armenia's critical infrastructure at the Information Systems Agency of Armenia.</t>
-  </si>
-  <si>
-    <t>https://sessionize.com/image/71f5-400o400o1-BVLaZdEqXxPwDdXZowmvfo.png</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="d MMM yyyy HH:mm AM/PM"/>
-    <numFmt numFmtId="165" formatCode="d mmm yyyy h:mm am/pm"/>
+    <numFmt numFmtId="164" formatCode="d mmm yyyy h:mm am/pm"/>
+    <numFmt numFmtId="165" formatCode="d MMM yyyy HH:mm AM/PM"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -417,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -433,11 +597,17 @@
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -445,13 +615,13 @@
     <xf borderId="2" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -738,7 +908,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4">
-        <v>1069411.0</v>
+        <v>1074683.0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>19</v>
@@ -753,13 +923,13 @@
         <v>22</v>
       </c>
       <c r="F2" s="5">
-        <v>45963.40416666667</v>
+        <v>45971.34027777778</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>23</v>
       </c>
       <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -781,13 +951,13 @@
       <c r="R2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4">
-        <v>1069557.0</v>
+        <v>1070707.0</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>30</v>
@@ -802,313 +972,579 @@
         <v>33</v>
       </c>
       <c r="F3" s="5">
-        <v>45963.40416666667</v>
+        <v>45964.65277777778</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="6"/>
+      <c r="H3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="5">
+        <v>46011.569444444445</v>
+      </c>
+      <c r="J3" s="4">
+        <v>30.0</v>
+      </c>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" s="8" t="s">
         <v>39</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9">
-        <v>1062404.0</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="A4" s="4">
+        <v>1070383.0</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="10">
-        <v>45953.493055555555</v>
-      </c>
-      <c r="G4" s="10">
-        <v>45953.50069444445</v>
-      </c>
-      <c r="H4" s="9" t="s">
+      <c r="E4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="11">
-        <v>46011.4375</v>
-      </c>
-      <c r="J4" s="9">
-        <v>120.0</v>
-      </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="9" t="s">
+      <c r="F4" s="5">
+        <v>45964.64444444444</v>
+      </c>
+      <c r="G4" s="5">
+        <v>45964.71805555555</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="I4" s="5">
+        <v>46011.52777777778</v>
+      </c>
+      <c r="J4" s="4">
+        <v>90.0</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="N4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="P4" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q4" s="9" t="s">
+      <c r="O4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="P4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="S4" s="13" t="s">
+      <c r="R4" s="4" t="s">
         <v>50</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="9">
-        <v>1064706.0</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="A5" s="4">
+        <v>1070100.0</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="10">
-        <v>45957.709027777775</v>
-      </c>
-      <c r="G5" s="11">
-        <v>45958.175</v>
-      </c>
-      <c r="H5" s="9" t="s">
+      <c r="E5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="11">
-        <v>46011.4375</v>
-      </c>
-      <c r="J5" s="9">
-        <v>30.0</v>
-      </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="9" t="s">
+      <c r="F5" s="5">
+        <v>45965.34861111111</v>
+      </c>
+      <c r="G5" s="5">
+        <v>45965.580555555556</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="N5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="O5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="P5" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q5" s="9" t="s">
+      <c r="P5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="R5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="S5" s="13" t="s">
+      <c r="S5" s="7" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="9">
-        <v>1060533.0</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="4">
+        <v>1069557.0</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="10">
-        <v>45951.566666666666</v>
-      </c>
-      <c r="G6" s="10">
-        <v>45951.575</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" s="10">
-        <v>46011.458333333336</v>
-      </c>
-      <c r="J6" s="9">
-        <v>30.0</v>
-      </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="9" t="s">
+      <c r="F6" s="8">
+        <v>45963.40416666667</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="N6" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="O6" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="P6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="Q6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="R6" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="S6" s="13" t="s">
+      <c r="S6" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="9">
-        <v>1066127.0</v>
-      </c>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="4">
+        <v>1069411.0</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="11">
-        <v>45959.54722222222</v>
-      </c>
-      <c r="G7" s="9" t="s">
+      <c r="F7" s="8">
+        <v>45963.40416666667</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I7" s="11">
-        <v>46011.479166666664</v>
-      </c>
-      <c r="J7" s="9">
-        <v>30.0</v>
-      </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="9" t="s">
+      <c r="H7" s="9"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="N7" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="O7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="P7" s="9" t="s">
+      <c r="P7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="Q7" s="9" t="s">
+      <c r="Q7" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="R7" s="9" t="s">
+      <c r="R7" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="S7" s="7" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="9">
+      <c r="A8" s="4">
+        <v>1066696.0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="5">
+        <v>45972.67291666667</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="11">
+        <v>1066127.0</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="12">
+        <v>45959.54722222222</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="12">
+        <v>46011.479166666664</v>
+      </c>
+      <c r="J9" s="11">
+        <v>30.0</v>
+      </c>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="P9" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q9" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="S9" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="11">
+        <v>1064706.0</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" s="15">
+        <v>45957.709027777775</v>
+      </c>
+      <c r="G10" s="12">
+        <v>45958.175</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="12">
+        <v>46011.4375</v>
+      </c>
+      <c r="J10" s="11">
+        <v>30.0</v>
+      </c>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q10" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="S10" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11">
+        <v>1062404.0</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="15">
+        <v>45953.493055555555</v>
+      </c>
+      <c r="G11" s="15">
+        <v>45953.50069444445</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="12">
+        <v>46011.4375</v>
+      </c>
+      <c r="J11" s="11">
+        <v>120.0</v>
+      </c>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="P11" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q11" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="R11" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="S11" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="11">
         <v>1061298.0</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F8" s="11">
+      <c r="B12" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F12" s="12">
         <v>45960.46875</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I8" s="11">
+      <c r="H12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="12">
         <v>46011.5</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J12" s="11">
         <v>10.0</v>
       </c>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="N8" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="P8" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q8" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="R8" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="S8" s="13" t="s">
-        <v>91</v>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="P12" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q12" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="S12" s="14" t="s">
+        <v>131</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" s="11">
+        <v>1060533.0</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" s="15">
+        <v>45951.566666666666</v>
+      </c>
+      <c r="G13" s="15">
+        <v>45951.575</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="15">
+        <v>46011.458333333336</v>
+      </c>
+      <c r="J13" s="11">
+        <v>30.0</v>
+      </c>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="P13" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q13" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="S13" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="17" ht="15.75" customHeight="1"/>
+    <row r="18" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1"/>
+    <row r="20" ht="15.75" customHeight="1"/>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
     <row r="25" ht="15.75" customHeight="1"/>
@@ -2080,15 +2516,6 @@
     <row r="991" ht="15.75" customHeight="1"/>
     <row r="992" ht="15.75" customHeight="1"/>
     <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
-    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="S2"/>
@@ -2098,10 +2525,15 @@
     <hyperlink r:id="rId5" ref="S6"/>
     <hyperlink r:id="rId6" ref="S7"/>
     <hyperlink r:id="rId7" ref="S8"/>
+    <hyperlink r:id="rId8" ref="S9"/>
+    <hyperlink r:id="rId9" ref="S10"/>
+    <hyperlink r:id="rId10" ref="S11"/>
+    <hyperlink r:id="rId11" ref="S12"/>
+    <hyperlink r:id="rId12" ref="S13"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId8"/>
+  <drawing r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add new sessions and speakers; include details for Gabriel Preda, Massoud Asadi, and Andrey Roshchupkin
</commit_message>
<xml_diff>
--- a/public/devfest-armenia-2025-flattened-sessions.xlsx
+++ b/public/devfest-armenia-2025-flattened-sessions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="173">
   <si>
     <t>Session Id</t>
   </si>
@@ -73,6 +73,123 @@
   </si>
   <si>
     <t>Profile Picture</t>
+  </si>
+  <si>
+    <t>Build products and services powered by Vertex AI, ADK, and Gemini</t>
+  </si>
+  <si>
+    <t>Discover how to build production-ready AI experiences with Vertex AI, the Agentic Development Kit (ADK), and Gemini—from first prompt to reliable API. We will show how you can combine the various agent patterns predefined in ADK with custom agents and tools to create powerful autonomous applications. As examples we will include a travel multi-agent application as well as an multi-source information retrieval application.</t>
+  </si>
+  <si>
+    <t>Gabriel Preda</t>
+  </si>
+  <si>
+    <t>gabi.preda@gmail.com</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Hall A</t>
+  </si>
+  <si>
+    <t>24806d60-f727-4328-9942-68684ecca775</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>Preda</t>
+  </si>
+  <si>
+    <t>Principal Data Scientist at Endava, Kaggle &amp; AI GDE, 2x Kaggle Grandmaster</t>
+  </si>
+  <si>
+    <t>Survived PhD in Computational Electromagnetics, while working as a researcher, applied 25 years ago what will be called now Machine Learning to solve ill-posed inverse problems in NDT, worked for long time in Software Development, with positions from developer to senior manager or programme manager, started few years ago to dive into Data Science, currently working as a Principal Data Scientist at Endava. Author with Packt of a book on Kaggle Notebooks (data analytics, machine learning, generative AI), 2x Kaggle Grandmaster, GDE for AI and Kaggle.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/62cf-400o400o1-X27bXbraTJw4fzuaAenybF.jpg</t>
+  </si>
+  <si>
+    <t>eBPF Explained: Architecture, Real-World Problems, and Practical Solutions</t>
+  </si>
+  <si>
+    <t>eBPF has quickly become one of the most exciting technologies in the Linux world, giving developers new ways to understand and control what’s happening inside their systems. In this talk, I’ll explain eBPF in simple, practical terms—what it is, why it matters, and how you can actually use it in real applications. I’ll walk through a small demo, show how to load and run eBPF programs from user space, and share the lessons I’ve learned while experimenting with networking and observability use cases. I’ll also highlight how Google uses eBPF in products like GKE and gVisor, and even parts of Android’s networking and security stack to solve real-world performance and security challenges. By the end, attendees will have a clear, realistic idea of how eBPF actually works and can help them debug, optimize, and better understand their own systems.
+ • Understand what eBPF is, how it works, and why it’s transforming modern Linux systems.
+ • Learn how to write, load, and run eBPF programs from user space with practical networking and observability examples.
+ • See how Google uses eBPF in GKE, gVisor, and Android—and how to apply these patterns in your own engineering work.
+ 0:00–2:00 — The problem: traditional networking &amp; observability limitations
+ 2:00–5:00 — What is eBPF? Why it exists, and what problems it solves
+ 5:00–9:00 — How eBPF works: maps, hooks, verifier, and program lifecycle
+ 9:00–15:00 — Demo: writing &amp; running a minimal eBPF program
+ 15:00–20:00 — Google’s usage: GKE, gVisor, Android networking
+ 20:00–24:00 — Practical guidance: integrating eBPF into your projects
+ 24:00–25:00 — Key lessons
+ 25:00–30:00 — Q&amp;A
+ Audience level: beginner to advance.
+ presentation language is English.
+ Tags: Android, DevOps, Security, Backend, Developer Experience
+ No prerequisites. Basic familiarity with Linux or networking is helpful but not required.</t>
+  </si>
+  <si>
+    <t>Massoud Asadi</t>
+  </si>
+  <si>
+    <t>massoud.asadi@hotmail.com</t>
+  </si>
+  <si>
+    <t>Hall B (Wokshops)</t>
+  </si>
+  <si>
+    <t>900d7922-1c84-4e75-93ff-b48d9b22062a</t>
+  </si>
+  <si>
+    <t>Massoud</t>
+  </si>
+  <si>
+    <t>Asadi</t>
+  </si>
+  <si>
+    <t>Senior Software Engineer at PharmaBits</t>
+  </si>
+  <si>
+    <t>I’m a Senior Software Engineer with over eight years of experience across backend, frontend, and system-level development. I’ve worked with distributed systems, high-performance .NET services, and modern web technologies, and more recently I’ve been exploring eBPF, system-level networking, and advanced observability tools. I also have hands-on experience with LLM integration and building AI-powered workflows. At PharmaBits, I work on backend architecture, developer tooling, and full-stack product features. I enjoy turning complex technical concepts into practical insights and look forward to sharing what I’ve learned with the DevFest Armenia community.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/f5c1-400o400o1-PwTj2qHiGx8Zb89eXmvD6r.jpg</t>
+  </si>
+  <si>
+    <t>WebAI in Action: AI-Powered Accessibility Testing in Chrome</t>
+  </si>
+  <si>
+    <t>Chrome’s built-in WebAI provides access to Gemini, a multimodal AI model that can analyze text, images, and web page structures directly in the browser. In this session, I’ll show how a QA engineer can use it to build a working Chrome extension for accessibility testing.
+ The tool combines visual and DOM analysis to detect accessibility issues and generate actionable recommendations — from color contrast improvements to labeling corrections — all running locally in Chrome using Gemini.
+ For the workshop, you can find the extension here: https://github.com/Andrey-Roshchupkin/chrome-web-ai-a11y-testing-extension
+ Note that the Gemini Nano model in Chrome and the Gemma model in Ollama will take some time to download, so it might be better to do this at home.</t>
+  </si>
+  <si>
+    <t>Andrey Roshchupkin</t>
+  </si>
+  <si>
+    <t>reivrn@gmail.com</t>
+  </si>
+  <si>
+    <t>3fbdb1ff-2d59-4b5b-abde-d76761a04412</t>
+  </si>
+  <si>
+    <t>Andrey</t>
+  </si>
+  <si>
+    <t>Roshchupkin</t>
+  </si>
+  <si>
+    <t>SDET in VL | Building AI-Powered Solutions</t>
+  </si>
+  <si>
+    <t>Andrey Roshchupkin is an SDET passionate about blending AI with software testing. He builds open, practical tools that help QA engineers adopt cutting-edge technologies like Chrome WebAI and Gemini to make testing smarter and more accessible. Beyond testing, he explores AI in creative applications, demonstrating how these technologies can solve real-world problems.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/e10b-400o400o1-W9qosLXaGyqKT5vDHPZXiM.png</t>
   </si>
   <si>
     <t>Simple Emotional Intelligence Skills [WORKSHOP]</t>
@@ -89,9 +206,6 @@
   </si>
   <si>
     <t>narefyeva.coach@gmail.com</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>fcd40625-d41f-45f8-8b4b-fc510bb96d07</t>
@@ -129,9 +243,6 @@
   </si>
   <si>
     <t>yoyu777@gmail.com</t>
-  </si>
-  <si>
-    <t>Hall A</t>
   </si>
   <si>
     <t>7fd4159e-a3e4-4ebf-93d9-62c78f7e8323</t>
@@ -844,7 +955,8 @@
     <col customWidth="1" min="2" max="2" width="89.0"/>
     <col customWidth="1" min="3" max="16" width="8.71"/>
     <col customWidth="1" min="17" max="17" width="48.14"/>
-    <col customWidth="1" min="18" max="26" width="8.71"/>
+    <col customWidth="1" min="18" max="18" width="34.43"/>
+    <col customWidth="1" min="19" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -908,7 +1020,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4">
-        <v>1074683.0</v>
+        <v>1078912.0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>19</v>
@@ -923,65 +1035,71 @@
         <v>22</v>
       </c>
       <c r="F2" s="5">
-        <v>45971.34027777778</v>
+        <v>45978.59583333333</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="H2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="5">
+        <v>46011.67361111111</v>
+      </c>
+      <c r="J2" s="4">
+        <v>30.0</v>
+      </c>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>22</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4">
-        <v>1070707.0</v>
+        <v>1077338.0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F3" s="5">
-        <v>45964.65277777778</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>23</v>
+        <v>45979.38888888889</v>
+      </c>
+      <c r="G3" s="5">
+        <v>45979.40416666667</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I3" s="5">
-        <v>46011.569444444445</v>
+        <v>46011.61111111111</v>
       </c>
       <c r="J3" s="4">
         <v>30.0</v>
@@ -989,57 +1107,57 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4">
-        <v>1070383.0</v>
+        <v>1076657.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F4" s="5">
-        <v>45964.64444444444</v>
+        <v>45978.59583333333</v>
       </c>
       <c r="G4" s="5">
-        <v>45964.71805555555</v>
+        <v>45978.62708333333</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="I4" s="5">
-        <v>46011.52777777778</v>
+        <v>46011.42361111111</v>
       </c>
       <c r="J4" s="4">
-        <v>90.0</v>
+        <v>30.0</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
@@ -1053,7 +1171,7 @@
         <v>48</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q4" s="4" t="s">
         <v>49</v>
@@ -1067,7 +1185,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4">
-        <v>1070100.0</v>
+        <v>1074683.0</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>52</v>
@@ -1082,10 +1200,10 @@
         <v>55</v>
       </c>
       <c r="F5" s="5">
-        <v>45965.34861111111</v>
-      </c>
-      <c r="G5" s="5">
-        <v>45965.580555555556</v>
+        <v>45971.34027777778</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -1116,7 +1234,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4">
-        <v>1069557.0</v>
+        <v>1070707.0</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>62</v>
@@ -1130,17 +1248,23 @@
       <c r="E6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="8">
-        <v>45963.40416666667</v>
+      <c r="F6" s="5">
+        <v>45964.65277777778</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
+      <c r="H6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="5">
+        <v>46011.569444444445</v>
+      </c>
+      <c r="J6" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
       <c r="M6" s="4" t="s">
         <v>66</v>
       </c>
@@ -1165,7 +1289,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4">
-        <v>1069411.0</v>
+        <v>1070383.0</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>72</v>
@@ -1179,60 +1303,66 @@
       <c r="E7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="8">
-        <v>45963.40416666667</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
+      <c r="F7" s="5">
+        <v>45964.64444444444</v>
+      </c>
+      <c r="G7" s="5">
+        <v>45964.71805555555</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="5">
+        <v>46011.52777777778</v>
+      </c>
+      <c r="J7" s="4">
+        <v>90.0</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
       <c r="M7" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="P7" s="4" t="s">
         <v>75</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4">
-        <v>1066696.0</v>
+        <v>1070100.0</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F8" s="5">
-        <v>45972.67291666667</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>23</v>
+        <v>45965.34861111111</v>
+      </c>
+      <c r="G8" s="5">
+        <v>45965.580555555556</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -1240,274 +1370,256 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="P8" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="N8" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="Q8" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="S8" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11">
-        <v>1066127.0</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" s="11" t="s">
+      <c r="A9" s="4">
+        <v>1069557.0</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="C9" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F9" s="12">
-        <v>45959.54722222222</v>
-      </c>
-      <c r="G9" s="11" t="s">
+      <c r="E9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="8">
+        <v>45963.40416666667</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="12">
-        <v>46011.479166666664</v>
-      </c>
-      <c r="J9" s="11">
-        <v>30.0</v>
-      </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="11" t="s">
+      <c r="H9" s="9"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="P9" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="N9" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="O9" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="P9" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q9" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="R9" s="11" t="s">
+      <c r="Q9" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="S9" s="14" t="s">
+      <c r="R9" s="4" t="s">
         <v>101</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="11">
-        <v>1064706.0</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="11" t="s">
+      <c r="A10" s="4">
+        <v>1069411.0</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="C10" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="D10" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F10" s="15">
-        <v>45957.709027777775</v>
-      </c>
-      <c r="G10" s="12">
-        <v>45958.175</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="12">
-        <v>46011.4375</v>
-      </c>
-      <c r="J10" s="11">
-        <v>30.0</v>
-      </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="11" t="s">
+      <c r="E10" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="N10" s="11" t="s">
+      <c r="F10" s="8">
+        <v>45963.40416666667</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="O10" s="11" t="s">
+      <c r="N10" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="P10" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q10" s="11" t="s">
+      <c r="O10" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="R10" s="11" t="s">
+      <c r="P10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q10" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="S10" s="14" t="s">
+      <c r="R10" s="4" t="s">
         <v>111</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="11">
-        <v>1062404.0</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C11" s="11" t="s">
+      <c r="A11" s="4">
+        <v>1066696.0</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="C11" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="D11" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="15">
-        <v>45953.493055555555</v>
-      </c>
-      <c r="G11" s="15">
-        <v>45953.50069444445</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" s="12">
-        <v>46011.4375</v>
-      </c>
-      <c r="J11" s="11">
-        <v>120.0</v>
-      </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="11" t="s">
+      <c r="E11" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="N11" s="11" t="s">
+      <c r="F11" s="5">
+        <v>45972.67291666667</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="O11" s="11" t="s">
+      <c r="N11" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="P11" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q11" s="11" t="s">
+      <c r="O11" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="R11" s="11" t="s">
+      <c r="P11" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q11" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="S11" s="14" t="s">
+      <c r="R11" s="4" t="s">
         <v>121</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="11">
-        <v>1061298.0</v>
+        <v>1066127.0</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F12" s="12">
-        <v>45960.46875</v>
+        <v>45959.54722222222</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>23</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I12" s="12">
-        <v>46011.5</v>
+        <v>46011.479166666664</v>
       </c>
       <c r="J12" s="11">
-        <v>10.0</v>
+        <v>30.0</v>
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="P12" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="N12" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="O12" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="P12" s="11" t="s">
-        <v>125</v>
-      </c>
       <c r="Q12" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="S12" s="14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="11">
-        <v>1060533.0</v>
+        <v>1064706.0</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F13" s="15">
-        <v>45951.566666666666</v>
-      </c>
-      <c r="G13" s="15">
-        <v>45951.575</v>
+        <v>45957.709027777775</v>
+      </c>
+      <c r="G13" s="12">
+        <v>45958.175</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="15">
-        <v>46011.458333333336</v>
+        <v>24</v>
+      </c>
+      <c r="I13" s="12">
+        <v>46011.4375</v>
       </c>
       <c r="J13" s="11">
         <v>30.0</v>
@@ -1515,30 +1627,192 @@
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="P13" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="N13" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="O13" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="P13" s="11" t="s">
-        <v>135</v>
-      </c>
       <c r="Q13" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="S13" s="14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="11">
+        <v>1062404.0</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="15">
+        <v>45953.493055555555</v>
+      </c>
+      <c r="G14" s="15">
+        <v>45953.50069444445</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="12">
+        <v>46011.4375</v>
+      </c>
+      <c r="J14" s="11">
+        <v>120.0</v>
+      </c>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="N14" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="O14" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="P14" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q14" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="S14" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="11">
+        <v>1061298.0</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" s="12">
+        <v>45960.46875</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="12">
+        <v>46011.5</v>
+      </c>
+      <c r="J15" s="11">
+        <v>10.0</v>
+      </c>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="P15" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q15" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="R15" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="S15" s="14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="11">
+        <v>1060533.0</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16" s="15">
+        <v>45951.566666666666</v>
+      </c>
+      <c r="G16" s="15">
+        <v>45951.575</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="15">
+        <v>46011.458333333336</v>
+      </c>
+      <c r="J16" s="11">
+        <v>30.0</v>
+      </c>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="N16" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="O16" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="P16" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q16" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="S16" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -2530,10 +2804,13 @@
     <hyperlink r:id="rId10" ref="S11"/>
     <hyperlink r:id="rId11" ref="S12"/>
     <hyperlink r:id="rId12" ref="S13"/>
+    <hyperlink r:id="rId13" ref="S14"/>
+    <hyperlink r:id="rId14" ref="S15"/>
+    <hyperlink r:id="rId15" ref="S16"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId13"/>
+  <drawing r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add new sessions and speakers; include details for Carlos Sanchez, Kevork Sulahian, Luiz Carneiro, Daniel Gonik, and Vardges Begoyan
</commit_message>
<xml_diff>
--- a/public/devfest-armenia-2025-flattened-sessions.xlsx
+++ b/public/devfest-armenia-2025-flattened-sessions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="223">
   <si>
     <t>Session Id</t>
   </si>
@@ -75,6 +75,139 @@
     <t>Profile Picture</t>
   </si>
   <si>
+    <t>Self-Healing Rollouts: Automating Production Fixes with Google Gemini and Google Jules</t>
+  </si>
+  <si>
+    <t>Even with robust CI/CD, production rollouts can hit unexpected snags. While in Kubernetes Argo Rollouts excels at Progressive Delivery and automated rollbacks to mitigate deployment issues, what if we could go a step further?
+ This session explores how to elevate your release process by integrating Agentic AI using Google Gemini and Google Jules, an Asynchronous Coding Agent, with Argo Rollouts canary deployments on GKE. We'll demonstrate how an intelligent agent can automatically analyze logs when a rollout fails, pinpointing the root cause. Beyond diagnosis, these agents can take proactive steps on your behalf, suggesting and even implementing code fixes as new pull requests, which can be redeployed automatically after PR review. This approach moves us closer to truly self-healing deployments.
+ Join us to learn how to combine the power of Kubernetes and Argo Rollouts with the autonomous capabilities of Agentic AI using Gemini and Google Jules, achieving a release experience that is not only seamless but also resilient.</t>
+  </si>
+  <si>
+    <t>Carlos Sanchez</t>
+  </si>
+  <si>
+    <t>carlos@csanchez.org</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Hall A</t>
+  </si>
+  <si>
+    <t>efce0e79-3d0c-47cf-98d2-1bb8884c1e10</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Sanchez</t>
+  </si>
+  <si>
+    <t>Principal Scientist at Adobe</t>
+  </si>
+  <si>
+    <t>Carlos Sanchez is a Principal Scientist at Adobe Experience Manager, specializing in software automation, from build tools to Continuous Delivery and Progressive Delivery. Involved in Open Source for over 20 years, he is the author of the Jenkins Kubernetes plugin and a member of the Apache Software Foundation amongst other open source groups, contributing to several projects, such as Kubernetes, Jenkins or Apache Maven.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/f0b0-400o400o1-9tUWwiZVmgtRM6Wi1AF7mw.png</t>
+  </si>
+  <si>
+    <t>Operationalizing Evaluations: Framework for Automated CI/CD in the era of Generative Models for LLMs</t>
+  </si>
+  <si>
+    <t>LLM applications break traditional testing: outputs are stochastic, non-deterministic, and impossible to validate with string-matching unit tests. This talk introduces a practical framework for “Semantic CI/CD,” where LLMs automatically evaluate other LLMs using robust, binary scoring—no humans and no heuristics. Building on findings from Gaming the Answer Matcher, we show that judge models are far more robust than commonly assumed and can act as reliable gatekeepers in production pipelines.</t>
+  </si>
+  <si>
+    <t>Kevork Sulahian</t>
+  </si>
+  <si>
+    <t>kevork.ysulahian@gmail.com</t>
+  </si>
+  <si>
+    <t>76de9ed8-afd1-499b-be1c-8cafae9585fe</t>
+  </si>
+  <si>
+    <t>Kevork</t>
+  </si>
+  <si>
+    <t>Sulahian</t>
+  </si>
+  <si>
+    <t>Staff ML Engineer &amp; AAAI author</t>
+  </si>
+  <si>
+    <t>Staff ML Engineer working on Gen AI application, LLM Safety and Evals</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/72df-400o400o1-BYDRKTYd36RySuy1Wi14rj.jpg</t>
+  </si>
+  <si>
+    <t>What candies are Agentic AI frameworks stealing from developers?</t>
+  </si>
+  <si>
+    <t>The rise of Agentic AI frameworks marks a profound change in software engineering, fundamentally shifting the boundary between what developers write and what a framework handles. But what, exactly, are these powerful frameworks automating away?
+ This provocative talk, "What candies are Agentic AI frameworks stealing from developers?", explores how modern Agentic frameworks abstract key parts of the system flow. We will clarify and reproduce core agent responsibilities, such as tool orchestration and the Agent control loop, demonstrating exactly how these are being absorbed by the framework. This is not just a high-level discussion; it is a practical lesson on framework design and architectural knowledge essential before building agents. By analyzing which "candies" are being "stolen," attendees will gain the clarity needed to focus their future skill development in where it's being expected that developers invest their craft.</t>
+  </si>
+  <si>
+    <t>Luiz Carneiro</t>
+  </si>
+  <si>
+    <t>luiz@carneiro.dev</t>
+  </si>
+  <si>
+    <t>2874dccd-57d6-4281-80ad-8c2461f7b957</t>
+  </si>
+  <si>
+    <t>Luiz</t>
+  </si>
+  <si>
+    <t>Carneiro</t>
+  </si>
+  <si>
+    <t>Phd, Solution Engineer @ smapiot</t>
+  </si>
+  <si>
+    <t>Luiz is an accomplished Cloud Engineer with extensive experience in scalable solutions and software development. His technical depth is uniquely underpinned by a strong background in research, holding a Ph.D. in Physics, which fuels his analytical approach to complex engineering challenges. Luiz closely follows the AI Engineering revolution, with a special dedication to AI agent systems architecture. Beyond his professional roles, he is a dedicated community leader, actively organizing the GDG Cloud Munich, a thriving developer group that fosters knowledge-sharing and networking in cloud technologies.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/d67a-400o400o1-aprDDPetxHDkvAPGcy8gGz.png</t>
+  </si>
+  <si>
+    <t>AI in Real Engineering Work: How to Build Fast in 2025 Without Creating Tomorrow’s Legacy</t>
+  </si>
+  <si>
+    <t>The talk explores how AI tools can dramatically speed up engineering work in 2025 while still avoiding the trap of creating “tomorrow’s legacy.” It focuses on where AI genuinely helps, boilerplate, testing, documentation, refactoring, and where human judgment is still essential for architecture, long-term decisions, and debugging. The goal is to give engineers a practical framework for building fast without sacrificing quality or maintainability.</t>
+  </si>
+  <si>
+    <t>Daniel Gonik</t>
+  </si>
+  <si>
+    <t>gonik.daniel88@gmail.com</t>
+  </si>
+  <si>
+    <t>Hall B (Wokshops)</t>
+  </si>
+  <si>
+    <t>94a1abff-8230-4ca3-b3cf-1937e2682cc8</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Gonik</t>
+  </si>
+  <si>
+    <t>Senior Software Engineer</t>
+  </si>
+  <si>
+    <t>As a Senior Fullstack Engineer and experienced Team Lead, I bring a wealth of experience in building and maintaining high-performance, user-friendly web applications. My passion for building tomorrow's applications and services for the web, combined with my expertise in React, Node (Express, Nest, Koa), Angular, HTML/CSS, preprocessors, webpack, and Git, enables me to deliver cutting-edge solutions that meet the needs of my clients. I also have a strong interest in new technologies, security, writing, and general hacking about.
+ I have a proven track record of leading and mentoring teams to success, and I am dedicated to constantly learning and improving in many IT-related topics, particularly JavaScript, React, Angular, NodeJS and many other *.JS technologies. I am confident that my skills and experience will add value to any organization and I am excited to bring my expertise to your company and help drive your business forward.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/a4c6-400o400o1-HJozpjEkFQ663xLnkkp4GJ.png</t>
+  </si>
+  <si>
     <t>Build products and services powered by Vertex AI, ADK, and Gemini</t>
   </si>
   <si>
@@ -85,12 +218,6 @@
   </si>
   <si>
     <t>gabi.preda@gmail.com</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Hall A</t>
   </si>
   <si>
     <t>24806d60-f727-4328-9942-68684ecca775</t>
@@ -138,9 +265,6 @@
     <t>massoud.asadi@hotmail.com</t>
   </si>
   <si>
-    <t>Hall B (Wokshops)</t>
-  </si>
-  <si>
     <t>900d7922-1c84-4e75-93ff-b48d9b22062a</t>
   </si>
   <si>
@@ -392,6 +516,43 @@
   </si>
   <si>
     <t>https://sessionize.com/image/0f4f-400o400o1-325zV56GBzG8KTAwZDjWyK.jpg</t>
+  </si>
+  <si>
+    <t>Building Software Like Buildings: Processes, Tests &amp; Structure</t>
+  </si>
+  <si>
+    <t>Too often, teams postpone discipline — processes, testing, and architecture — until it’s too late. But just like buildings, software needs strong foundations from the start. In this talk, I’ll share why early processes (planning, code freeze, retrospectives), meaningful unit tests, and aligned architecture matter for both startups and large companies. Using real industry cases and a building analogy, we’ll explore how skipping these leads to unstable “floors,” technical debt, and lost users. Attendees will leave with practical insights on introducing discipline early without slowing down innovation.
+ Takeaways
+ Why early processes (planning, reviews, releases) prevent chaos later.
+ How meaningful unit tests and quality gates protect core functionality.
+ Why scalable architecture and standards are critical for growth - even in small teams.
+ Language: EN
+ Prerequisites:
+ General knowledge of agile/scrum practices and software development life cycle.</t>
+  </si>
+  <si>
+    <t>Vardges Begoyan</t>
+  </si>
+  <si>
+    <t>vardges.begoyan@gmail.com</t>
+  </si>
+  <si>
+    <t>1054eb16-3c55-46a5-bacd-7f6195dc31ed</t>
+  </si>
+  <si>
+    <t>Vardges</t>
+  </si>
+  <si>
+    <t>Begoyan</t>
+  </si>
+  <si>
+    <t>IT Governance SDLC Manager, Ameriabank</t>
+  </si>
+  <si>
+    <t>I am SDLC Manager in IT Governance of Ameriabank with a strong background in leading engineering teams and defining best practices across the software development lifecycle. I am passionate about translating technical discipline into tangible business impact, supporting engineering excellence at both macro (governance and processes) and micro (code quality, team practices) levels. My mission is to help organizations build software foundations that are stable, scalable, and resilient.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/84d1-400o400o1-EmdTSdSmp9VsjvUjU3EN6n.jpg</t>
   </si>
   <si>
     <t>Engineering Leadership for Distributed Teams: Balancing Code, People, and Culture</t>
@@ -1020,7 +1181,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4">
-        <v>1078912.0</v>
+        <v>1084075.0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>19</v>
@@ -1035,7 +1196,7 @@
         <v>22</v>
       </c>
       <c r="F2" s="5">
-        <v>45978.59583333333</v>
+        <v>45987.30972222222</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>23</v>
@@ -1044,7 +1205,7 @@
         <v>24</v>
       </c>
       <c r="I2" s="5">
-        <v>46011.67361111111</v>
+        <v>46011.72222222222</v>
       </c>
       <c r="J2" s="4">
         <v>30.0</v>
@@ -1075,7 +1236,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4">
-        <v>1077338.0</v>
+        <v>1083992.0</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>31</v>
@@ -1090,16 +1251,16 @@
         <v>34</v>
       </c>
       <c r="F3" s="5">
-        <v>45979.38888888889</v>
+        <v>45987.30972222222</v>
       </c>
       <c r="G3" s="5">
-        <v>45979.40416666667</v>
+        <v>45987.37152777778</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="I3" s="5">
-        <v>46011.61111111111</v>
+        <v>46011.57638888889</v>
       </c>
       <c r="J3" s="4">
         <v>30.0</v>
@@ -1107,54 +1268,54 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>34</v>
       </c>
       <c r="Q3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4">
-        <v>1076657.0</v>
+        <v>1081873.0</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="F4" s="5">
-        <v>45978.59583333333</v>
-      </c>
-      <c r="G4" s="5">
-        <v>45978.62708333333</v>
+        <v>45982.60625</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="I4" s="5">
-        <v>46011.42361111111</v>
+        <v>46011.680555555555</v>
       </c>
       <c r="J4" s="4">
         <v>30.0</v>
@@ -1162,52 +1323,58 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="P4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="S4" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4">
-        <v>1074683.0</v>
+        <v>1080232.0</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="5">
+        <v>45982.43125</v>
+      </c>
+      <c r="G5" s="5">
+        <v>45982.479166666664</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="5">
-        <v>45971.34027777778</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+      <c r="I5" s="5">
+        <v>46011.631944444445</v>
+      </c>
+      <c r="J5" s="4">
+        <v>30.0</v>
+      </c>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
       <c r="M5" s="4" t="s">
@@ -1220,7 +1387,7 @@
         <v>58</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q5" s="4" t="s">
         <v>59</v>
@@ -1234,7 +1401,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4">
-        <v>1070707.0</v>
+        <v>1078912.0</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>62</v>
@@ -1249,7 +1416,7 @@
         <v>65</v>
       </c>
       <c r="F6" s="5">
-        <v>45964.65277777778</v>
+        <v>45978.59583333333</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>23</v>
@@ -1258,7 +1425,7 @@
         <v>24</v>
       </c>
       <c r="I6" s="5">
-        <v>46011.569444444445</v>
+        <v>46011.67361111111</v>
       </c>
       <c r="J6" s="4">
         <v>30.0</v>
@@ -1289,7 +1456,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4">
-        <v>1070383.0</v>
+        <v>1077338.0</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>72</v>
@@ -1304,216 +1471,234 @@
         <v>75</v>
       </c>
       <c r="F7" s="5">
-        <v>45964.64444444444</v>
+        <v>45979.38888888889</v>
       </c>
       <c r="G7" s="5">
-        <v>45964.71805555555</v>
+        <v>45979.40416666667</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="I7" s="5">
-        <v>46011.52777777778</v>
+        <v>46011.61111111111</v>
       </c>
       <c r="J7" s="4">
-        <v>90.0</v>
+        <v>30.0</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="N7" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="O7" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="P7" s="4" t="s">
         <v>75</v>
       </c>
       <c r="Q7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="R7" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="S7" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="S7" s="7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4">
-        <v>1070100.0</v>
+        <v>1076657.0</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="F8" s="5">
-        <v>45965.34861111111</v>
+        <v>45978.59583333333</v>
       </c>
       <c r="G8" s="5">
-        <v>45965.580555555556</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
+        <v>45978.62708333333</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="5">
+        <v>46011.42361111111</v>
+      </c>
+      <c r="J8" s="4">
+        <v>30.0</v>
+      </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="N8" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="P8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q8" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="P8" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q8" s="4" t="s">
+      <c r="R8" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="R8" s="4" t="s">
+      <c r="S8" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="S8" s="7" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4">
-        <v>1069557.0</v>
+        <v>1074683.0</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F9" s="8">
-        <v>45963.40416666667</v>
+      <c r="F9" s="5">
+        <v>45971.34027777778</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
       <c r="M9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="N9" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="O9" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="P9" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q9" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="P9" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q9" s="4" t="s">
+      <c r="R9" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="S9" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="S9" s="7" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4">
-        <v>1069411.0</v>
+        <v>1070707.0</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="8">
-        <v>45963.40416666667</v>
+      <c r="F10" s="5">
+        <v>45964.65277777778</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="H10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="5">
+        <v>46011.569444444445</v>
+      </c>
+      <c r="J10" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
       <c r="M10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="N10" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="O10" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="P10" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q10" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="P10" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q10" s="4" t="s">
+      <c r="R10" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="R10" s="4" t="s">
+      <c r="S10" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="S10" s="7" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4">
-        <v>1066696.0</v>
+        <v>1070383.0</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="5">
+        <v>45964.64444444444</v>
+      </c>
+      <c r="G11" s="5">
+        <v>45964.71805555555</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F11" s="5">
-        <v>45972.67291666667</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+      <c r="I11" s="5">
+        <v>46011.52777777778</v>
+      </c>
+      <c r="J11" s="4">
+        <v>90.0</v>
+      </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="4" t="s">
@@ -1526,7 +1711,7 @@
         <v>119</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q11" s="4" t="s">
         <v>120</v>
@@ -1539,285 +1724,531 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="11">
-        <v>1066127.0</v>
-      </c>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="4">
+        <v>1070100.0</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F12" s="12">
-        <v>45959.54722222222</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="12">
-        <v>46011.479166666664</v>
-      </c>
-      <c r="J12" s="11">
-        <v>30.0</v>
-      </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="11" t="s">
+      <c r="F12" s="5">
+        <v>45965.34861111111</v>
+      </c>
+      <c r="G12" s="5">
+        <v>45965.580555555556</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="N12" s="11" t="s">
+      <c r="N12" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="O12" s="11" t="s">
+      <c r="O12" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="P12" s="11" t="s">
+      <c r="P12" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="Q12" s="11" t="s">
+      <c r="Q12" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="R12" s="11" t="s">
+      <c r="R12" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="S12" s="14" t="s">
+      <c r="S12" s="7" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11">
-        <v>1064706.0</v>
-      </c>
-      <c r="B13" s="11" t="s">
+      <c r="A13" s="4">
+        <v>1069557.0</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="15">
-        <v>45957.709027777775</v>
-      </c>
-      <c r="G13" s="12">
-        <v>45958.175</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="12">
-        <v>46011.4375</v>
-      </c>
-      <c r="J13" s="11">
-        <v>30.0</v>
-      </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="11" t="s">
+      <c r="F13" s="8">
+        <v>45963.40416666667</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="N13" s="11" t="s">
+      <c r="N13" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="O13" s="11" t="s">
+      <c r="O13" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="P13" s="11" t="s">
+      <c r="P13" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="Q13" s="11" t="s">
+      <c r="Q13" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="R13" s="11" t="s">
+      <c r="R13" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="S13" s="14" t="s">
+      <c r="S13" s="7" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="11">
-        <v>1062404.0</v>
-      </c>
-      <c r="B14" s="11" t="s">
+      <c r="A14" s="4">
+        <v>1069411.0</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="15">
-        <v>45953.493055555555</v>
-      </c>
-      <c r="G14" s="15">
-        <v>45953.50069444445</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" s="12">
-        <v>46011.4375</v>
-      </c>
-      <c r="J14" s="11">
-        <v>120.0</v>
-      </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="11" t="s">
+      <c r="F14" s="8">
+        <v>45963.40416666667</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="N14" s="11" t="s">
+      <c r="N14" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="O14" s="11" t="s">
+      <c r="O14" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="P14" s="11" t="s">
+      <c r="P14" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="Q14" s="11" t="s">
+      <c r="Q14" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="R14" s="11" t="s">
+      <c r="R14" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="S14" s="14" t="s">
+      <c r="S14" s="7" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="11">
-        <v>1061298.0</v>
-      </c>
-      <c r="B15" s="11" t="s">
+      <c r="A15" s="4">
+        <v>1066927.0</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="F15" s="12">
-        <v>45960.46875</v>
-      </c>
-      <c r="G15" s="11" t="s">
+      <c r="F15" s="5">
+        <v>45965.34861111111</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="12">
-        <v>46011.5</v>
-      </c>
-      <c r="J15" s="11">
-        <v>10.0</v>
-      </c>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="11" t="s">
+      <c r="I15" s="5">
+        <v>46011.65972222222</v>
+      </c>
+      <c r="J15" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="N15" s="11" t="s">
+      <c r="N15" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="O15" s="11" t="s">
+      <c r="O15" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="P15" s="11" t="s">
+      <c r="P15" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="Q15" s="11" t="s">
+      <c r="Q15" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="R15" s="11" t="s">
+      <c r="R15" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="S15" s="14" t="s">
+      <c r="S15" s="7" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="11">
+      <c r="A16" s="4">
+        <v>1066696.0</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16" s="5">
+        <v>45972.67291666667</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="11">
+        <v>1066127.0</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="F17" s="12">
+        <v>45959.54722222222</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="12">
+        <v>46011.479166666664</v>
+      </c>
+      <c r="J17" s="11">
+        <v>30.0</v>
+      </c>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="P17" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q17" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="R17" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="S17" s="14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="11">
+        <v>1064706.0</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="F18" s="15">
+        <v>45957.709027777775</v>
+      </c>
+      <c r="G18" s="12">
+        <v>45958.175</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="12">
+        <v>46011.4375</v>
+      </c>
+      <c r="J18" s="11">
+        <v>30.0</v>
+      </c>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="O18" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="P18" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q18" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="R18" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="S18" s="14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="11">
+        <v>1062404.0</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F19" s="15">
+        <v>45953.493055555555</v>
+      </c>
+      <c r="G19" s="15">
+        <v>45953.50069444445</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="I19" s="12">
+        <v>46011.4375</v>
+      </c>
+      <c r="J19" s="11">
+        <v>120.0</v>
+      </c>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="N19" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="O19" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="P19" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q19" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="R19" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="S19" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="11">
+        <v>1061298.0</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="F20" s="12">
+        <v>45960.46875</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="12">
+        <v>46011.5</v>
+      </c>
+      <c r="J20" s="11">
+        <v>10.0</v>
+      </c>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="N20" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="O20" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="P20" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q20" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="R20" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="S20" s="14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="11">
         <v>1060533.0</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="F16" s="15">
+      <c r="B21" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F21" s="15">
         <v>45951.566666666666</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G21" s="15">
         <v>45951.575</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H21" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I21" s="15">
         <v>46011.458333333336</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J21" s="11">
         <v>30.0</v>
       </c>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="N16" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="O16" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="P16" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q16" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="R16" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="S16" s="14" t="s">
-        <v>172</v>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="N21" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="O21" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="P21" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q21" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="R21" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="S21" s="14" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
@@ -2807,10 +3238,15 @@
     <hyperlink r:id="rId13" ref="S14"/>
     <hyperlink r:id="rId14" ref="S15"/>
     <hyperlink r:id="rId15" ref="S16"/>
+    <hyperlink r:id="rId16" ref="S17"/>
+    <hyperlink r:id="rId17" ref="S18"/>
+    <hyperlink r:id="rId18" ref="S19"/>
+    <hyperlink r:id="rId19" ref="S20"/>
+    <hyperlink r:id="rId20" ref="S21"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId16"/>
+  <drawing r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add new sessions and speakers; include details for Rouben Meschian. Added schedule
</commit_message>
<xml_diff>
--- a/public/devfest-armenia-2025-flattened-sessions.xlsx
+++ b/public/devfest-armenia-2025-flattened-sessions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="233">
   <si>
     <t>Session Id</t>
   </si>
@@ -73,6 +73,39 @@
   </si>
   <si>
     <t>Profile Picture</t>
+  </si>
+  <si>
+    <t>Programming Practices for Developing Quality Software</t>
+  </si>
+  <si>
+    <t>This is a brain dump of some lessons learned while developing software over the past 20 years.</t>
+  </si>
+  <si>
+    <t>Rouben Meschian</t>
+  </si>
+  <si>
+    <t>rmeschian@gmail.com</t>
+  </si>
+  <si>
+    <t>Hall A</t>
+  </si>
+  <si>
+    <t>a0956f01-5704-4386-85b3-ee6d65565ec0</t>
+  </si>
+  <si>
+    <t>Rouben</t>
+  </si>
+  <si>
+    <t>Meschian</t>
+  </si>
+  <si>
+    <t>Software Engineer | Educator</t>
+  </si>
+  <si>
+    <t>Rouben has collaborated extensively with numerous companies, demonstrating a strong passion for developing solutions that address enterprise challenges. With a solid background in distributed systems, he has devoted much of his career to building scalable web applications.</t>
+  </si>
+  <si>
+    <t>https://sessionize.com/image/154d-400o400o1-UtPakgM8JvwMm99ALBmoBw.jpg</t>
   </si>
   <si>
     <t>Self-Healing Rollouts: Automating Production Fixes with Google Gemini and Google Jules</t>
@@ -90,9 +123,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>Hall A</t>
   </si>
   <si>
     <t>efce0e79-3d0c-47cf-98d2-1bb8884c1e10</t>
@@ -1181,7 +1211,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4">
-        <v>1084075.0</v>
+        <v>1086335.0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>19</v>
@@ -1196,16 +1226,16 @@
         <v>22</v>
       </c>
       <c r="F2" s="5">
-        <v>45987.30972222222</v>
-      </c>
-      <c r="G2" s="4" t="s">
+        <v>45991.3375</v>
+      </c>
+      <c r="G2" s="5">
+        <v>45991.39166666667</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="I2" s="5">
-        <v>46011.72222222222</v>
+        <v>46011.493055555555</v>
       </c>
       <c r="J2" s="4">
         <v>30.0</v>
@@ -1213,54 +1243,54 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>22</v>
       </c>
       <c r="Q2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4">
-        <v>1083992.0</v>
+        <v>1084075.0</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="F3" s="5">
         <v>45987.30972222222</v>
       </c>
-      <c r="G3" s="5">
-        <v>45987.37152777778</v>
+      <c r="G3" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" s="5">
-        <v>46011.57638888889</v>
+        <v>46011.72222222222</v>
       </c>
       <c r="J3" s="4">
         <v>30.0</v>
@@ -1277,7 +1307,7 @@
         <v>37</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>38</v>
@@ -1291,7 +1321,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4">
-        <v>1081873.0</v>
+        <v>1083992.0</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>41</v>
@@ -1306,16 +1336,16 @@
         <v>44</v>
       </c>
       <c r="F4" s="5">
-        <v>45982.60625</v>
-      </c>
-      <c r="G4" s="4" t="s">
+        <v>45987.30972222222</v>
+      </c>
+      <c r="G4" s="5">
+        <v>45987.37152777778</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="I4" s="5">
-        <v>46011.680555555555</v>
+        <v>46011.57638888889</v>
       </c>
       <c r="J4" s="4">
         <v>30.0</v>
@@ -1346,7 +1376,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4">
-        <v>1080232.0</v>
+        <v>1081873.0</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>51</v>
@@ -1361,16 +1391,16 @@
         <v>54</v>
       </c>
       <c r="F5" s="5">
-        <v>45982.43125</v>
-      </c>
-      <c r="G5" s="5">
-        <v>45982.479166666664</v>
+        <v>45982.60625</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="I5" s="5">
-        <v>46011.631944444445</v>
+        <v>46011.680555555555</v>
       </c>
       <c r="J5" s="4">
         <v>30.0</v>
@@ -1378,54 +1408,54 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
       <c r="M5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="P5" s="4" t="s">
         <v>54</v>
       </c>
       <c r="Q5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="S5" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="S5" s="7" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4">
-        <v>1078912.0</v>
+        <v>1080232.0</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="5">
+        <v>45982.43125</v>
+      </c>
+      <c r="G6" s="5">
+        <v>45982.479166666664</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="5">
-        <v>45978.59583333333</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="I6" s="5">
-        <v>46011.67361111111</v>
+        <v>46011.631944444445</v>
       </c>
       <c r="J6" s="4">
         <v>30.0</v>
@@ -1442,7 +1472,7 @@
         <v>68</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q6" s="4" t="s">
         <v>69</v>
@@ -1456,7 +1486,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4">
-        <v>1077338.0</v>
+        <v>1078912.0</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>72</v>
@@ -1471,16 +1501,16 @@
         <v>75</v>
       </c>
       <c r="F7" s="5">
-        <v>45979.38888888889</v>
-      </c>
-      <c r="G7" s="5">
-        <v>45979.40416666667</v>
+        <v>45978.59583333333</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="I7" s="5">
-        <v>46011.61111111111</v>
+        <v>46011.67361111111</v>
       </c>
       <c r="J7" s="4">
         <v>30.0</v>
@@ -1511,7 +1541,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4">
-        <v>1076657.0</v>
+        <v>1077338.0</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>82</v>
@@ -1526,16 +1556,16 @@
         <v>85</v>
       </c>
       <c r="F8" s="5">
-        <v>45978.59583333333</v>
+        <v>45979.38888888889</v>
       </c>
       <c r="G8" s="5">
-        <v>45978.62708333333</v>
+        <v>45979.40416666667</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="I8" s="5">
-        <v>46011.42361111111</v>
+        <v>46011.61111111111</v>
       </c>
       <c r="J8" s="4">
         <v>30.0</v>
@@ -1566,7 +1596,7 @@
     </row>
     <row r="9">
       <c r="A9" s="4">
-        <v>1074683.0</v>
+        <v>1076657.0</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>92</v>
@@ -1581,14 +1611,20 @@
         <v>95</v>
       </c>
       <c r="F9" s="5">
-        <v>45971.34027777778</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+        <v>45978.59583333333</v>
+      </c>
+      <c r="G9" s="5">
+        <v>45978.62708333333</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="5">
+        <v>46011.42361111111</v>
+      </c>
+      <c r="J9" s="4">
+        <v>30.0</v>
+      </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="4" t="s">
@@ -1615,7 +1651,7 @@
     </row>
     <row r="10">
       <c r="A10" s="4">
-        <v>1070707.0</v>
+        <v>1074683.0</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>102</v>
@@ -1630,20 +1666,14 @@
         <v>105</v>
       </c>
       <c r="F10" s="5">
-        <v>45964.65277777778</v>
+        <v>45971.34027777778</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="5">
-        <v>46011.569444444445</v>
-      </c>
-      <c r="J10" s="4">
-        <v>30.0</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="4" t="s">
@@ -1670,7 +1700,7 @@
     </row>
     <row r="11">
       <c r="A11" s="4">
-        <v>1070383.0</v>
+        <v>1070707.0</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>112</v>
@@ -1685,69 +1715,75 @@
         <v>115</v>
       </c>
       <c r="F11" s="5">
-        <v>45964.64444444444</v>
-      </c>
-      <c r="G11" s="5">
-        <v>45964.71805555555</v>
+        <v>45964.65277777778</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>116</v>
+        <v>23</v>
       </c>
       <c r="I11" s="5">
-        <v>46011.52777777778</v>
+        <v>46011.569444444445</v>
       </c>
       <c r="J11" s="4">
-        <v>90.0</v>
+        <v>30.0</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="N11" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="O11" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>119</v>
       </c>
       <c r="P11" s="4" t="s">
         <v>115</v>
       </c>
       <c r="Q11" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="R11" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="S11" s="7" t="s">
         <v>121</v>
-      </c>
-      <c r="S11" s="7" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4">
-        <v>1070100.0</v>
+        <v>1070383.0</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="5">
+        <v>45964.64444444444</v>
+      </c>
+      <c r="G12" s="5">
+        <v>45964.71805555555</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F12" s="5">
-        <v>45965.34861111111</v>
-      </c>
-      <c r="G12" s="5">
-        <v>45965.580555555556</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="I12" s="5">
+        <v>46011.52777777778</v>
+      </c>
+      <c r="J12" s="4">
+        <v>90.0</v>
+      </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="4" t="s">
@@ -1760,7 +1796,7 @@
         <v>129</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q12" s="4" t="s">
         <v>130</v>
@@ -1774,7 +1810,7 @@
     </row>
     <row r="13">
       <c r="A13" s="4">
-        <v>1069557.0</v>
+        <v>1070100.0</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>133</v>
@@ -1788,17 +1824,17 @@
       <c r="E13" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="8">
-        <v>45963.40416666667</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
+      <c r="F13" s="5">
+        <v>45965.34861111111</v>
+      </c>
+      <c r="G13" s="5">
+        <v>45965.580555555556</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
       <c r="M13" s="4" t="s">
         <v>137</v>
       </c>
@@ -1823,7 +1859,7 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="4">
-        <v>1069411.0</v>
+        <v>1069557.0</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>143</v>
@@ -1841,7 +1877,7 @@
         <v>45963.40416666667</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="10"/>
@@ -1872,7 +1908,7 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="4">
-        <v>1066927.0</v>
+        <v>1069411.0</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>153</v>
@@ -1886,23 +1922,17 @@
       <c r="E15" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="F15" s="5">
-        <v>45965.34861111111</v>
+      <c r="F15" s="8">
+        <v>45963.40416666667</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" s="5">
-        <v>46011.65972222222</v>
-      </c>
-      <c r="J15" s="4">
-        <v>30.0</v>
-      </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
       <c r="M15" s="4" t="s">
         <v>157</v>
       </c>
@@ -1927,7 +1957,7 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="4">
-        <v>1066696.0</v>
+        <v>1066927.0</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>163</v>
@@ -1942,14 +1972,20 @@
         <v>166</v>
       </c>
       <c r="F16" s="5">
-        <v>45972.67291666667</v>
+        <v>45965.34861111111</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
+      <c r="I16" s="5">
+        <v>46011.65972222222</v>
+      </c>
+      <c r="J16" s="4">
+        <v>30.0</v>
+      </c>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="4" t="s">
@@ -1975,63 +2011,57 @@
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="11">
-        <v>1066127.0</v>
-      </c>
-      <c r="B17" s="11" t="s">
+      <c r="A17" s="4">
+        <v>1066696.0</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F17" s="12">
-        <v>45959.54722222222</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I17" s="12">
-        <v>46011.479166666664</v>
-      </c>
-      <c r="J17" s="11">
-        <v>30.0</v>
-      </c>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="11" t="s">
+      <c r="F17" s="5">
+        <v>45972.67291666667</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="N17" s="11" t="s">
+      <c r="N17" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="O17" s="11" t="s">
+      <c r="O17" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="P17" s="11" t="s">
+      <c r="P17" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="Q17" s="11" t="s">
+      <c r="Q17" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="R17" s="11" t="s">
+      <c r="R17" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="S17" s="14" t="s">
+      <c r="S17" s="7" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="11">
-        <v>1064706.0</v>
+        <v>1066127.0</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>183</v>
@@ -2045,17 +2075,17 @@
       <c r="E18" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="F18" s="15">
-        <v>45957.709027777775</v>
-      </c>
-      <c r="G18" s="12">
-        <v>45958.175</v>
+      <c r="F18" s="12">
+        <v>45959.54722222222</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I18" s="12">
-        <v>46011.4375</v>
+        <v>46011.479166666664</v>
       </c>
       <c r="J18" s="11">
         <v>30.0</v>
@@ -2086,7 +2116,7 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="11">
-        <v>1062404.0</v>
+        <v>1064706.0</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>193</v>
@@ -2101,19 +2131,19 @@
         <v>196</v>
       </c>
       <c r="F19" s="15">
-        <v>45953.493055555555</v>
-      </c>
-      <c r="G19" s="15">
-        <v>45953.50069444445</v>
+        <v>45957.709027777775</v>
+      </c>
+      <c r="G19" s="12">
+        <v>45958.175</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>116</v>
+        <v>23</v>
       </c>
       <c r="I19" s="12">
         <v>46011.4375</v>
       </c>
       <c r="J19" s="11">
-        <v>120.0</v>
+        <v>30.0</v>
       </c>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
@@ -2141,7 +2171,7 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="11">
-        <v>1061298.0</v>
+        <v>1062404.0</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>203</v>
@@ -2155,20 +2185,20 @@
       <c r="E20" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="F20" s="12">
-        <v>45960.46875</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>23</v>
+      <c r="F20" s="15">
+        <v>45953.493055555555</v>
+      </c>
+      <c r="G20" s="15">
+        <v>45953.50069444445</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="I20" s="12">
-        <v>46011.5</v>
+        <v>46011.4375</v>
       </c>
       <c r="J20" s="11">
-        <v>10.0</v>
+        <v>120.0</v>
       </c>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
@@ -2196,7 +2226,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="11">
-        <v>1060533.0</v>
+        <v>1061298.0</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>213</v>
@@ -2210,20 +2240,20 @@
       <c r="E21" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="F21" s="15">
-        <v>45951.566666666666</v>
-      </c>
-      <c r="G21" s="15">
-        <v>45951.575</v>
+      <c r="F21" s="12">
+        <v>45960.46875</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I21" s="15">
-        <v>46011.458333333336</v>
+        <v>23</v>
+      </c>
+      <c r="I21" s="12">
+        <v>46011.5</v>
       </c>
       <c r="J21" s="11">
-        <v>30.0</v>
+        <v>10.0</v>
       </c>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
@@ -2249,7 +2279,61 @@
         <v>222</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="11">
+        <v>1060533.0</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="F22" s="15">
+        <v>45951.566666666666</v>
+      </c>
+      <c r="G22" s="15">
+        <v>45951.575</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="15">
+        <v>46011.458333333336</v>
+      </c>
+      <c r="J22" s="11">
+        <v>30.0</v>
+      </c>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="O22" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="P22" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q22" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="R22" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="S22" s="14" t="s">
+        <v>232</v>
+      </c>
+    </row>
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
     <row r="25" ht="15.75" customHeight="1"/>
@@ -3243,10 +3327,11 @@
     <hyperlink r:id="rId18" ref="S19"/>
     <hyperlink r:id="rId19" ref="S20"/>
     <hyperlink r:id="rId20" ref="S21"/>
+    <hyperlink r:id="rId21" ref="S22"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId21"/>
+  <drawing r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>